<commit_message>
Added TC_Summary Excel file
</commit_message>
<xml_diff>
--- a/Docs/TC_Summary.xlsx
+++ b/Docs/TC_Summary.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E596"/>
+  <dimension ref="A1:E604"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10523,176 +10523,176 @@
     </row>
     <row r="404">
       <c r="A404" s="2" t="n">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B404" s="3" t="inlineStr">
         <is>
-          <t>Device Discovery Test Plan</t>
+          <t xml:space="preserve">Smoke CO Alarm </t>
         </is>
       </c>
       <c r="C404" s="3" t="inlineStr">
         <is>
-          <t>[TC-DD-1.1] QR Code Onboarding Payload Verification [DUT - Commissionee]</t>
+          <t>[TC-SMOKECO-1.1] Global attributes with DUT as Server</t>
         </is>
       </c>
       <c r="D404" s="3" t="inlineStr">
         <is>
-          <t>TC-DD-1.1</t>
+          <t>TC-SMOKECO-1.1</t>
         </is>
       </c>
       <c r="E404" s="2" t="inlineStr">
         <is>
-          <t>Core Test Case</t>
+          <t>App Test Case</t>
         </is>
       </c>
     </row>
     <row r="405">
       <c r="A405" s="2" t="n">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B405" s="3" t="inlineStr">
         <is>
-          <t>Device Discovery Test Plan</t>
+          <t xml:space="preserve">Smoke CO Alarm </t>
         </is>
       </c>
       <c r="C405" s="3" t="inlineStr">
         <is>
-          <t>[TC-DD-1.2] Manual Pairing Code Payload Verification [DUT - Commissionee]</t>
+          <t>[TC-SMOKECO-2.1] Attributes with DUT as Server</t>
         </is>
       </c>
       <c r="D405" s="3" t="inlineStr">
         <is>
-          <t>TC-DD-1.2</t>
+          <t>TC-SMOKECO-2.1</t>
         </is>
       </c>
       <c r="E405" s="2" t="inlineStr">
         <is>
-          <t>Core Test Case</t>
+          <t>App Test Case</t>
         </is>
       </c>
     </row>
     <row r="406">
       <c r="A406" s="2" t="n">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B406" s="3" t="inlineStr">
         <is>
-          <t>Device Discovery Test Plan</t>
+          <t xml:space="preserve">Smoke CO Alarm </t>
         </is>
       </c>
       <c r="C406" s="3" t="inlineStr">
         <is>
-          <t>[TC-DD-1.3] NFC Onboarding Payload Verification [DUT - Commissionee] - REMOVED</t>
+          <t>[TC-SMOKECO-2.2] Primary Functionality - Smoke Alarm with DUT as Server</t>
         </is>
       </c>
       <c r="D406" s="3" t="inlineStr">
         <is>
-          <t>TC-DD-1.3</t>
+          <t>TC-SMOKECO-2.2</t>
         </is>
       </c>
       <c r="E406" s="2" t="inlineStr">
         <is>
-          <t>Core Test Case</t>
+          <t>App Test Case</t>
         </is>
       </c>
     </row>
     <row r="407">
       <c r="A407" s="2" t="n">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B407" s="3" t="inlineStr">
         <is>
-          <t>Device Discovery Test Plan</t>
+          <t xml:space="preserve">Smoke CO Alarm </t>
         </is>
       </c>
       <c r="C407" s="3" t="inlineStr">
         <is>
-          <t>[TC-DD-1.4] Concatenation - QR Code Onboarding Payload Verification [DUT - Commissionee] - REMOVED</t>
+          <t>[TC-SMOKECO-2.3] Primary Functionality - CO Alarm with DUT as Server</t>
         </is>
       </c>
       <c r="D407" s="3" t="inlineStr">
         <is>
-          <t>TC-DD-1.4</t>
+          <t>TC-SMOKECO-2.3</t>
         </is>
       </c>
       <c r="E407" s="2" t="inlineStr">
         <is>
-          <t>Core Test Case</t>
+          <t>App Test Case</t>
         </is>
       </c>
     </row>
     <row r="408">
       <c r="A408" s="2" t="n">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B408" s="3" t="inlineStr">
         <is>
-          <t>Device Discovery Test Plan</t>
+          <t xml:space="preserve">Smoke CO Alarm </t>
         </is>
       </c>
       <c r="C408" s="3" t="inlineStr">
         <is>
-          <t>[TC-DD-1.5] NFC Rules of Advertisement and Onboarding [DUT - Commissionee] - REMOVED</t>
+          <t>[TC-SMOKECO-2.4] Secondary Functionality - Mandatory with DUT as Server</t>
         </is>
       </c>
       <c r="D408" s="3" t="inlineStr">
         <is>
-          <t>TC-DD-1.5</t>
+          <t>TC-SMOKECO-2.4</t>
         </is>
       </c>
       <c r="E408" s="2" t="inlineStr">
         <is>
-          <t>Core Test Case</t>
+          <t>App Test Case</t>
         </is>
       </c>
     </row>
     <row r="409">
       <c r="A409" s="2" t="n">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B409" s="3" t="inlineStr">
         <is>
-          <t>Device Discovery Test Plan</t>
+          <t xml:space="preserve">Smoke CO Alarm </t>
         </is>
       </c>
       <c r="C409" s="3" t="inlineStr">
         <is>
-          <t>[TC-DD-1.6] QR Code Format and Label [DUT - Commissionee]</t>
+          <t>[TC-SMOKECO-2.5] Secondary Functionality - Optional with DUT as Server</t>
         </is>
       </c>
       <c r="D409" s="3" t="inlineStr">
         <is>
-          <t>TC-DD-1.6</t>
+          <t>TC-SMOKECO-2.5</t>
         </is>
       </c>
       <c r="E409" s="2" t="inlineStr">
         <is>
-          <t>Core Test Case</t>
+          <t>App Test Case</t>
         </is>
       </c>
     </row>
     <row r="410">
       <c r="A410" s="2" t="n">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B410" s="3" t="inlineStr">
         <is>
-          <t>Device Discovery Test Plan</t>
+          <t xml:space="preserve">Smoke CO Alarm </t>
         </is>
       </c>
       <c r="C410" s="3" t="inlineStr">
         <is>
-          <t>[TC-DD-1.7] Setup Code Format and Label [DUT - Commissionee]</t>
+          <t>[TC-SMOKECO-2.6] ExpressedState Attribute - Multiple Alarms with DUT as Server</t>
         </is>
       </c>
       <c r="D410" s="3" t="inlineStr">
         <is>
-          <t>TC-DD-1.7</t>
+          <t>TC-SMOKECO-2.6</t>
         </is>
       </c>
       <c r="E410" s="2" t="inlineStr">
         <is>
-          <t>Core Test Case</t>
+          <t>App Test Case</t>
         </is>
       </c>
     </row>
@@ -10707,12 +10707,12 @@
       </c>
       <c r="C411" s="3" t="inlineStr">
         <is>
-          <t>[TC-DD-1.8] QR Code Onboarding Payload Verification [DUT - Commissioner]</t>
+          <t>[TC-DD-1.1] QR Code Onboarding Payload Verification [DUT - Commissionee]</t>
         </is>
       </c>
       <c r="D411" s="3" t="inlineStr">
         <is>
-          <t>TC-DD-1.8</t>
+          <t>TC-DD-1.1</t>
         </is>
       </c>
       <c r="E411" s="2" t="inlineStr">
@@ -10732,12 +10732,12 @@
       </c>
       <c r="C412" s="3" t="inlineStr">
         <is>
-          <t>[TC-DD-1.9] Manual Pairing Code Payload Verification [DUT - Commissioner]</t>
+          <t>[TC-DD-1.2] Manual Pairing Code Payload Verification [DUT - Commissionee]</t>
         </is>
       </c>
       <c r="D412" s="3" t="inlineStr">
         <is>
-          <t>TC-DD-1.9</t>
+          <t>TC-DD-1.2</t>
         </is>
       </c>
       <c r="E412" s="2" t="inlineStr">
@@ -10757,12 +10757,12 @@
       </c>
       <c r="C413" s="3" t="inlineStr">
         <is>
-          <t>[TC-DD-1.10] NFC Onboarding Payload Verification [DUT - Commissioner] - REMOVED</t>
+          <t>[TC-DD-1.3] NFC Onboarding Payload Verification [DUT - Commissionee] - REMOVED</t>
         </is>
       </c>
       <c r="D413" s="3" t="inlineStr">
         <is>
-          <t>TC-DD-1.10</t>
+          <t>TC-DD-1.3</t>
         </is>
       </c>
       <c r="E413" s="2" t="inlineStr">
@@ -10782,12 +10782,12 @@
       </c>
       <c r="C414" s="3" t="inlineStr">
         <is>
-          <t>[TC-DD-1.11] Concatenation - QR Code Onboarding Payload Verification [DUT - Commissioner] - REMOVED</t>
+          <t>[TC-DD-1.4] Concatenation - QR Code Onboarding Payload Verification [DUT - Commissionee] - REMOVED</t>
         </is>
       </c>
       <c r="D414" s="3" t="inlineStr">
         <is>
-          <t>TC-DD-1.11</t>
+          <t>TC-DD-1.4</t>
         </is>
       </c>
       <c r="E414" s="2" t="inlineStr">
@@ -10807,12 +10807,12 @@
       </c>
       <c r="C415" s="3" t="inlineStr">
         <is>
-          <t>[TC-DD-1.12] Onboarding Payload Verification - Custom Flow = 0 [DUT - Commissionee]</t>
+          <t>[TC-DD-1.5] NFC Rules of Advertisement and Onboarding [DUT - Commissionee] - REMOVED</t>
         </is>
       </c>
       <c r="D415" s="3" t="inlineStr">
         <is>
-          <t>TC-DD-1.12</t>
+          <t>TC-DD-1.5</t>
         </is>
       </c>
       <c r="E415" s="2" t="inlineStr">
@@ -10832,12 +10832,12 @@
       </c>
       <c r="C416" s="3" t="inlineStr">
         <is>
-          <t>[TC-DD-1.13] Onboarding Payload Verification - Custom Flow = 1 [DUT - Commissionee]</t>
+          <t>[TC-DD-1.6] QR Code Format and Label [DUT - Commissionee]</t>
         </is>
       </c>
       <c r="D416" s="3" t="inlineStr">
         <is>
-          <t>TC-DD-1.13</t>
+          <t>TC-DD-1.6</t>
         </is>
       </c>
       <c r="E416" s="2" t="inlineStr">
@@ -10857,12 +10857,12 @@
       </c>
       <c r="C417" s="3" t="inlineStr">
         <is>
-          <t>[TC-DD-1.14] Onboarding Payload Verification - Custom Flow = 2 [DUT - Commissionee]</t>
+          <t>[TC-DD-1.7] Setup Code Format and Label [DUT - Commissionee]</t>
         </is>
       </c>
       <c r="D417" s="3" t="inlineStr">
         <is>
-          <t>TC-DD-1.14</t>
+          <t>TC-DD-1.7</t>
         </is>
       </c>
       <c r="E417" s="2" t="inlineStr">
@@ -10882,12 +10882,12 @@
       </c>
       <c r="C418" s="3" t="inlineStr">
         <is>
-          <t>[TC-DD-1.15] Onboarding Payload Verification - Unique Discriminator and Passcode Values [DUT - Commissionee]</t>
+          <t>[TC-DD-1.8] QR Code Onboarding Payload Verification [DUT - Commissioner]</t>
         </is>
       </c>
       <c r="D418" s="3" t="inlineStr">
         <is>
-          <t>TC-DD-1.15</t>
+          <t>TC-DD-1.8</t>
         </is>
       </c>
       <c r="E418" s="2" t="inlineStr">
@@ -10907,12 +10907,12 @@
       </c>
       <c r="C419" s="3" t="inlineStr">
         <is>
-          <t>[TC-DD-2.1] Announcement by Device Verification [DUT - Commissionee]</t>
+          <t>[TC-DD-1.9] Manual Pairing Code Payload Verification [DUT - Commissioner]</t>
         </is>
       </c>
       <c r="D419" s="3" t="inlineStr">
         <is>
-          <t>TC-DD-2.1</t>
+          <t>TC-DD-1.9</t>
         </is>
       </c>
       <c r="E419" s="2" t="inlineStr">
@@ -10932,12 +10932,12 @@
       </c>
       <c r="C420" s="3" t="inlineStr">
         <is>
-          <t>[TC-DD-2.2] Discovery by Commissioner Verification [DUT - Commissioner]</t>
+          <t>[TC-DD-1.10] NFC Onboarding Payload Verification [DUT - Commissioner] - REMOVED</t>
         </is>
       </c>
       <c r="D420" s="3" t="inlineStr">
         <is>
-          <t>TC-DD-2.2</t>
+          <t>TC-DD-1.10</t>
         </is>
       </c>
       <c r="E420" s="2" t="inlineStr">
@@ -10957,12 +10957,12 @@
       </c>
       <c r="C421" s="3" t="inlineStr">
         <is>
-          <t>[TC-DD-3.1] Commissioning Flow - Concurrent [DUT - Commissionee]</t>
+          <t>[TC-DD-1.11] Concatenation - QR Code Onboarding Payload Verification [DUT - Commissioner] - REMOVED</t>
         </is>
       </c>
       <c r="D421" s="3" t="inlineStr">
         <is>
-          <t>TC-DD-3.1</t>
+          <t>TC-DD-1.11</t>
         </is>
       </c>
       <c r="E421" s="2" t="inlineStr">
@@ -10982,12 +10982,12 @@
       </c>
       <c r="C422" s="3" t="inlineStr">
         <is>
-          <t>[TC-DD-3.2] Commissioning Flow - Non-concurrent [DUT - Commissionee] - REMOVED</t>
+          <t>[TC-DD-1.12] Onboarding Payload Verification - Custom Flow = 0 [DUT - Commissionee]</t>
         </is>
       </c>
       <c r="D422" s="3" t="inlineStr">
         <is>
-          <t>TC-DD-3.2</t>
+          <t>TC-DD-1.12</t>
         </is>
       </c>
       <c r="E422" s="2" t="inlineStr">
@@ -11007,12 +11007,12 @@
       </c>
       <c r="C423" s="3" t="inlineStr">
         <is>
-          <t>[TC-DD-3.3] User Directed Commissioning [DUT - Commissionee]</t>
+          <t>[TC-DD-1.13] Onboarding Payload Verification - Custom Flow = 1 [DUT - Commissionee]</t>
         </is>
       </c>
       <c r="D423" s="3" t="inlineStr">
         <is>
-          <t>TC-DD-3.3</t>
+          <t>TC-DD-1.13</t>
         </is>
       </c>
       <c r="E423" s="2" t="inlineStr">
@@ -11032,12 +11032,12 @@
       </c>
       <c r="C424" s="3" t="inlineStr">
         <is>
-          <t>[TC-DD-3.4] User Directed Commissioning [DUT - Commissioner]</t>
+          <t>[TC-DD-1.14] Onboarding Payload Verification - Custom Flow = 2 [DUT - Commissionee]</t>
         </is>
       </c>
       <c r="D424" s="3" t="inlineStr">
         <is>
-          <t>TC-DD-3.4</t>
+          <t>TC-DD-1.14</t>
         </is>
       </c>
       <c r="E424" s="2" t="inlineStr">
@@ -11057,12 +11057,12 @@
       </c>
       <c r="C425" s="3" t="inlineStr">
         <is>
-          <t>[TC-DD-3.5] Commissioning Flow - Concurrent [DUT - Commissioner]</t>
+          <t>[TC-DD-1.15] Onboarding Payload Verification - Unique Discriminator and Passcode Values [DUT - Commissionee]</t>
         </is>
       </c>
       <c r="D425" s="3" t="inlineStr">
         <is>
-          <t>TC-DD-3.5</t>
+          <t>TC-DD-1.15</t>
         </is>
       </c>
       <c r="E425" s="2" t="inlineStr">
@@ -11082,12 +11082,12 @@
       </c>
       <c r="C426" s="3" t="inlineStr">
         <is>
-          <t>[TC-DD-3.6] Commissioning Flow - Non-concurrent [DUT - Commissioner] - REMOVED</t>
+          <t>[TC-DD-2.1] Announcement by Device Verification [DUT - Commissionee]</t>
         </is>
       </c>
       <c r="D426" s="3" t="inlineStr">
         <is>
-          <t>TC-DD-3.6</t>
+          <t>TC-DD-2.1</t>
         </is>
       </c>
       <c r="E426" s="2" t="inlineStr">
@@ -11107,12 +11107,12 @@
       </c>
       <c r="C427" s="3" t="inlineStr">
         <is>
-          <t>[TC-DD-3.7] Commissioning Flow - Concurrent - Negative Scenario [DUT - Commissioner] - REMOVED</t>
+          <t>[TC-DD-2.2] Discovery by Commissioner Verification [DUT - Commissioner]</t>
         </is>
       </c>
       <c r="D427" s="3" t="inlineStr">
         <is>
-          <t>TC-DD-3.7</t>
+          <t>TC-DD-2.2</t>
         </is>
       </c>
       <c r="E427" s="2" t="inlineStr">
@@ -11132,12 +11132,12 @@
       </c>
       <c r="C428" s="3" t="inlineStr">
         <is>
-          <t>[TC-DD-3.8] Commissioning Flow - Non-concurrent - Negative Scenario [DUT - Commissioner] - REMOVED</t>
+          <t>[TC-DD-3.1] Commissioning Flow - Concurrent [DUT - Commissionee]</t>
         </is>
       </c>
       <c r="D428" s="3" t="inlineStr">
         <is>
-          <t>TC-DD-3.8</t>
+          <t>TC-DD-3.1</t>
         </is>
       </c>
       <c r="E428" s="2" t="inlineStr">
@@ -11157,12 +11157,12 @@
       </c>
       <c r="C429" s="3" t="inlineStr">
         <is>
-          <t>[TC-DD-3.9] Commissioning Flow - Custom Flow = 2 [DUT - Commissionee]</t>
+          <t>[TC-DD-3.2] Commissioning Flow - Non-concurrent [DUT - Commissionee] - REMOVED</t>
         </is>
       </c>
       <c r="D429" s="3" t="inlineStr">
         <is>
-          <t>TC-DD-3.9</t>
+          <t>TC-DD-3.2</t>
         </is>
       </c>
       <c r="E429" s="2" t="inlineStr">
@@ -11182,12 +11182,12 @@
       </c>
       <c r="C430" s="3" t="inlineStr">
         <is>
-          <t>[TC-DD-3.10] Commissioning Flow - Custom Flow = 2 [DUT - Commissioner]</t>
+          <t>[TC-DD-3.3] User Directed Commissioning [DUT - Commissionee]</t>
         </is>
       </c>
       <c r="D430" s="3" t="inlineStr">
         <is>
-          <t>TC-DD-3.10</t>
+          <t>TC-DD-3.3</t>
         </is>
       </c>
       <c r="E430" s="2" t="inlineStr">
@@ -11207,12 +11207,12 @@
       </c>
       <c r="C431" s="3" t="inlineStr">
         <is>
-          <t>[TC-DD-3.11] Commissioning Flow = 0 (Standard Flow) - QR Code [DUT - Commissioner]</t>
+          <t>[TC-DD-3.4] User Directed Commissioning [DUT - Commissioner]</t>
         </is>
       </c>
       <c r="D431" s="3" t="inlineStr">
         <is>
-          <t>TC-DD-3.11</t>
+          <t>TC-DD-3.4</t>
         </is>
       </c>
       <c r="E431" s="2" t="inlineStr">
@@ -11232,12 +11232,12 @@
       </c>
       <c r="C432" s="3" t="inlineStr">
         <is>
-          <t>[TC-DD-3.12] Commissioning Flow = 1 (User-Intent Flow) - QR Code [DUT - Commissioner]</t>
+          <t>[TC-DD-3.5] Commissioning Flow - Concurrent [DUT - Commissioner]</t>
         </is>
       </c>
       <c r="D432" s="3" t="inlineStr">
         <is>
-          <t>TC-DD-3.12</t>
+          <t>TC-DD-3.5</t>
         </is>
       </c>
       <c r="E432" s="2" t="inlineStr">
@@ -11257,12 +11257,12 @@
       </c>
       <c r="C433" s="3" t="inlineStr">
         <is>
-          <t>[TC-DD-3.13] Commissioning Flow = 2 (Custom Flow) - QR Code [DUT - Commissioner]</t>
+          <t>[TC-DD-3.6] Commissioning Flow - Non-concurrent [DUT - Commissioner] - REMOVED</t>
         </is>
       </c>
       <c r="D433" s="3" t="inlineStr">
         <is>
-          <t>TC-DD-3.13</t>
+          <t>TC-DD-3.6</t>
         </is>
       </c>
       <c r="E433" s="2" t="inlineStr">
@@ -11282,12 +11282,12 @@
       </c>
       <c r="C434" s="3" t="inlineStr">
         <is>
-          <t>[TC-DD-3.14] Commissioning Flow - QR Code - Negative Scenario [DUT - Commissioner]</t>
+          <t>[TC-DD-3.7] Commissioning Flow - Concurrent - Negative Scenario [DUT - Commissioner] - REMOVED</t>
         </is>
       </c>
       <c r="D434" s="3" t="inlineStr">
         <is>
-          <t>TC-DD-3.14</t>
+          <t>TC-DD-3.7</t>
         </is>
       </c>
       <c r="E434" s="2" t="inlineStr">
@@ -11307,12 +11307,12 @@
       </c>
       <c r="C435" s="3" t="inlineStr">
         <is>
-          <t>[TC-DD-3.15] Commissioning Flow - Manual Pairing Code [DUT - Commissioner]</t>
+          <t>[TC-DD-3.8] Commissioning Flow - Non-concurrent - Negative Scenario [DUT - Commissioner] - REMOVED</t>
         </is>
       </c>
       <c r="D435" s="3" t="inlineStr">
         <is>
-          <t>TC-DD-3.15</t>
+          <t>TC-DD-3.8</t>
         </is>
       </c>
       <c r="E435" s="2" t="inlineStr">
@@ -11332,12 +11332,12 @@
       </c>
       <c r="C436" s="3" t="inlineStr">
         <is>
-          <t>[TC-DD-3.16] Commissioning Flow - 11-digit Manual Pairing Code - Negative Scenario [DUT - Commissioner]</t>
+          <t>[TC-DD-3.9] Commissioning Flow - Custom Flow = 2 [DUT - Commissionee]</t>
         </is>
       </c>
       <c r="D436" s="3" t="inlineStr">
         <is>
-          <t>TC-DD-3.16</t>
+          <t>TC-DD-3.9</t>
         </is>
       </c>
       <c r="E436" s="2" t="inlineStr">
@@ -11357,12 +11357,12 @@
       </c>
       <c r="C437" s="3" t="inlineStr">
         <is>
-          <t>[TC-DD-3.17] Commissioning Flow - 21-digit Manual Pairing Code - Negative Scenario [DUT - Commissioner]</t>
+          <t>[TC-DD-3.10] Commissioning Flow - Custom Flow = 2 [DUT - Commissioner]</t>
         </is>
       </c>
       <c r="D437" s="3" t="inlineStr">
         <is>
-          <t>TC-DD-3.17</t>
+          <t>TC-DD-3.10</t>
         </is>
       </c>
       <c r="E437" s="2" t="inlineStr">
@@ -11382,12 +11382,12 @@
       </c>
       <c r="C438" s="3" t="inlineStr">
         <is>
-          <t>[TC-DD-3.18] Commissioning Flow - Commissioning Multiple Devices [DUT - Commissioner]</t>
+          <t>[TC-DD-3.11] Commissioning Flow = 0 (Standard Flow) - QR Code [DUT - Commissioner]</t>
         </is>
       </c>
       <c r="D438" s="3" t="inlineStr">
         <is>
-          <t>TC-DD-3.18</t>
+          <t>TC-DD-3.11</t>
         </is>
       </c>
       <c r="E438" s="2" t="inlineStr">
@@ -11407,12 +11407,12 @@
       </c>
       <c r="C439" s="3" t="inlineStr">
         <is>
-          <t>[TC-DD-3.19] Commissioning Flow - Commission, Unpair and Re-commission Device [DUT - Commissionee]</t>
+          <t>[TC-DD-3.12] Commissioning Flow = 1 (User-Intent Flow) - QR Code [DUT - Commissioner]</t>
         </is>
       </c>
       <c r="D439" s="3" t="inlineStr">
         <is>
-          <t>TC-DD-3.19</t>
+          <t>TC-DD-3.12</t>
         </is>
       </c>
       <c r="E439" s="2" t="inlineStr">
@@ -11432,12 +11432,12 @@
       </c>
       <c r="C440" s="3" t="inlineStr">
         <is>
-          <t>[TC-DD-3.20] Commissioning Flow - Commission, Unpair and Re-commission Device [DUT - Commissioner]</t>
+          <t>[TC-DD-3.13] Commissioning Flow = 2 (Custom Flow) - QR Code [DUT - Commissioner]</t>
         </is>
       </c>
       <c r="D440" s="3" t="inlineStr">
         <is>
-          <t>TC-DD-3.20</t>
+          <t>TC-DD-3.13</t>
         </is>
       </c>
       <c r="E440" s="2" t="inlineStr">
@@ -11457,12 +11457,12 @@
       </c>
       <c r="C441" s="3" t="inlineStr">
         <is>
-          <t>[TC-DD-3.21] Commissioning Flow - Commission Multiple-Endpoint Device [DUT - Commissioner]</t>
+          <t>[TC-DD-3.14] Commissioning Flow - QR Code - Negative Scenario [DUT - Commissioner]</t>
         </is>
       </c>
       <c r="D441" s="3" t="inlineStr">
         <is>
-          <t>TC-DD-3.21</t>
+          <t>TC-DD-3.14</t>
         </is>
       </c>
       <c r="E441" s="2" t="inlineStr">
@@ -11477,17 +11477,17 @@
       </c>
       <c r="B442" s="3" t="inlineStr">
         <is>
-          <t>Basic Information Test Plan</t>
+          <t>Device Discovery Test Plan</t>
         </is>
       </c>
       <c r="C442" s="3" t="inlineStr">
         <is>
-          <t>[TC-BINFO-1.1] Global Attributes with DUT as Server</t>
+          <t>[TC-DD-3.15] Commissioning Flow - Manual Pairing Code [DUT - Commissioner]</t>
         </is>
       </c>
       <c r="D442" s="3" t="inlineStr">
         <is>
-          <t>TC-BINFO-1.1</t>
+          <t>TC-DD-3.15</t>
         </is>
       </c>
       <c r="E442" s="2" t="inlineStr">
@@ -11502,17 +11502,17 @@
       </c>
       <c r="B443" s="3" t="inlineStr">
         <is>
-          <t>Basic Information Test Plan</t>
+          <t>Device Discovery Test Plan</t>
         </is>
       </c>
       <c r="C443" s="3" t="inlineStr">
         <is>
-          <t>[TC-BINFO-2.1] Attributes [DUT-Server]</t>
+          <t>[TC-DD-3.16] Commissioning Flow - 11-digit Manual Pairing Code - Negative Scenario [DUT - Commissioner]</t>
         </is>
       </c>
       <c r="D443" s="3" t="inlineStr">
         <is>
-          <t>TC-BINFO-2.1</t>
+          <t>TC-DD-3.16</t>
         </is>
       </c>
       <c r="E443" s="2" t="inlineStr">
@@ -11527,17 +11527,17 @@
       </c>
       <c r="B444" s="3" t="inlineStr">
         <is>
-          <t>Basic Information Test Plan</t>
+          <t>Device Discovery Test Plan</t>
         </is>
       </c>
       <c r="C444" s="3" t="inlineStr">
         <is>
-          <t>[TC-BINFO-2.2] Events [DUT-Server]</t>
+          <t>[TC-DD-3.17] Commissioning Flow - 21-digit Manual Pairing Code - Negative Scenario [DUT - Commissioner]</t>
         </is>
       </c>
       <c r="D444" s="3" t="inlineStr">
         <is>
-          <t>TC-BINFO-2.2</t>
+          <t>TC-DD-3.17</t>
         </is>
       </c>
       <c r="E444" s="2" t="inlineStr">
@@ -11552,17 +11552,17 @@
       </c>
       <c r="B445" s="3" t="inlineStr">
         <is>
-          <t>Basic Information Test Plan</t>
+          <t>Device Discovery Test Plan</t>
         </is>
       </c>
       <c r="C445" s="3" t="inlineStr">
         <is>
-          <t>[TC-BINFO-3.1] Appearance Attribute DUT as Server</t>
+          <t>[TC-DD-3.18] Commissioning Flow - Commissioning Multiple Devices [DUT - Commissioner]</t>
         </is>
       </c>
       <c r="D445" s="3" t="inlineStr">
         <is>
-          <t>TC-BINFO-3.1</t>
+          <t>TC-DD-3.18</t>
         </is>
       </c>
       <c r="E445" s="2" t="inlineStr">
@@ -11577,17 +11577,17 @@
       </c>
       <c r="B446" s="3" t="inlineStr">
         <is>
-          <t>Node Operational Credentials Test Plan</t>
+          <t>Device Discovery Test Plan</t>
         </is>
       </c>
       <c r="C446" s="3" t="inlineStr">
         <is>
-          <t>[TC-OPCREDS-1.2] Global Attributes with DUT as Server</t>
+          <t>[TC-DD-3.19] Commissioning Flow - Commission, Unpair and Re-commission Device [DUT - Commissionee]</t>
         </is>
       </c>
       <c r="D446" s="3" t="inlineStr">
         <is>
-          <t>TC-OPCREDS-1.2</t>
+          <t>TC-DD-3.19</t>
         </is>
       </c>
       <c r="E446" s="2" t="inlineStr">
@@ -11602,17 +11602,17 @@
       </c>
       <c r="B447" s="3" t="inlineStr">
         <is>
-          <t>Node Operational Credentials Test Plan</t>
+          <t>Device Discovery Test Plan</t>
         </is>
       </c>
       <c r="C447" s="3" t="inlineStr">
         <is>
-          <t>[TC-OPCREDS-3.1] Attribute-NOCs, TrustedRootCertificates list validation [DUT-Server]</t>
+          <t>[TC-DD-3.20] Commissioning Flow - Commission, Unpair and Re-commission Device [DUT - Commissioner]</t>
         </is>
       </c>
       <c r="D447" s="3" t="inlineStr">
         <is>
-          <t>TC-OPCREDS-3.1</t>
+          <t>TC-DD-3.20</t>
         </is>
       </c>
       <c r="E447" s="2" t="inlineStr">
@@ -11627,17 +11627,17 @@
       </c>
       <c r="B448" s="3" t="inlineStr">
         <is>
-          <t>Node Operational Credentials Test Plan</t>
+          <t>Device Discovery Test Plan</t>
         </is>
       </c>
       <c r="C448" s="3" t="inlineStr">
         <is>
-          <t>[TC-OPCREDS-3.2] Attribute-CurrentFabricIndex validation [DUT-Server]</t>
+          <t>[TC-DD-3.21] Commissioning Flow - Commission Multiple-Endpoint Device [DUT - Commissioner]</t>
         </is>
       </c>
       <c r="D448" s="3" t="inlineStr">
         <is>
-          <t>TC-OPCREDS-3.2</t>
+          <t>TC-DD-3.21</t>
         </is>
       </c>
       <c r="E448" s="2" t="inlineStr">
@@ -11652,17 +11652,17 @@
       </c>
       <c r="B449" s="3" t="inlineStr">
         <is>
-          <t>Node Operational Credentials Test Plan</t>
+          <t>Basic Information Test Plan</t>
         </is>
       </c>
       <c r="C449" s="3" t="inlineStr">
         <is>
-          <t>[TC-OPCREDS-3.4] UpdateNOC-Error Condition [DUT-Server]</t>
+          <t>[TC-BINFO-1.1] Global Attributes with DUT as Server</t>
         </is>
       </c>
       <c r="D449" s="3" t="inlineStr">
         <is>
-          <t>TC-OPCREDS-3.4</t>
+          <t>TC-BINFO-1.1</t>
         </is>
       </c>
       <c r="E449" s="2" t="inlineStr">
@@ -11677,17 +11677,17 @@
       </c>
       <c r="B450" s="3" t="inlineStr">
         <is>
-          <t>Node Operational Credentials Test Plan</t>
+          <t>Basic Information Test Plan</t>
         </is>
       </c>
       <c r="C450" s="3" t="inlineStr">
         <is>
-          <t>[TC-OPCREDS-3.5] NOC Check for UpdateNOC [DUT-Server]</t>
+          <t>[TC-BINFO-2.1] Attributes [DUT-Server]</t>
         </is>
       </c>
       <c r="D450" s="3" t="inlineStr">
         <is>
-          <t>TC-OPCREDS-3.5</t>
+          <t>TC-BINFO-2.1</t>
         </is>
       </c>
       <c r="E450" s="2" t="inlineStr">
@@ -11702,17 +11702,17 @@
       </c>
       <c r="B451" s="3" t="inlineStr">
         <is>
-          <t>Node Operational Credentials Test Plan</t>
+          <t>Basic Information Test Plan</t>
         </is>
       </c>
       <c r="C451" s="3" t="inlineStr">
         <is>
-          <t>[TC-OPCREDS-3.6] Last Fabric removal validation [DUT-Server]</t>
+          <t>[TC-BINFO-2.2] Events [DUT-Server]</t>
         </is>
       </c>
       <c r="D451" s="3" t="inlineStr">
         <is>
-          <t>TC-OPCREDS-3.6</t>
+          <t>TC-BINFO-2.2</t>
         </is>
       </c>
       <c r="E451" s="2" t="inlineStr">
@@ -11727,17 +11727,17 @@
       </c>
       <c r="B452" s="3" t="inlineStr">
         <is>
-          <t>Node Operational Credentials Test Plan</t>
+          <t>Basic Information Test Plan</t>
         </is>
       </c>
       <c r="C452" s="3" t="inlineStr">
         <is>
-          <t>[TC-OPCREDS-3.7] Add Second Fabric over CASE [DUT-Server]</t>
+          <t>[TC-BINFO-3.1] Appearance Attribute DUT as Server</t>
         </is>
       </c>
       <c r="D452" s="3" t="inlineStr">
         <is>
-          <t>TC-OPCREDS-3.7</t>
+          <t>TC-BINFO-3.1</t>
         </is>
       </c>
       <c r="E452" s="2" t="inlineStr">
@@ -11757,12 +11757,12 @@
       </c>
       <c r="C453" s="3" t="inlineStr">
         <is>
-          <t>[TC-OPCREDS-3.3] Attribute-NOCs, Commands [DUT-Client]</t>
+          <t>[TC-OPCREDS-1.2] Global Attributes with DUT as Server</t>
         </is>
       </c>
       <c r="D453" s="3" t="inlineStr">
         <is>
-          <t>TC-OPCREDS-3.3</t>
+          <t>TC-OPCREDS-1.2</t>
         </is>
       </c>
       <c r="E453" s="2" t="inlineStr">
@@ -11777,17 +11777,17 @@
       </c>
       <c r="B454" s="3" t="inlineStr">
         <is>
-          <t>Network Commissioning Test Plan</t>
+          <t>Node Operational Credentials Test Plan</t>
         </is>
       </c>
       <c r="C454" s="3" t="inlineStr">
         <is>
-          <t>[TC-CNET-1.3] Global Attributes with DUT as Server</t>
+          <t>[TC-OPCREDS-3.1] Attribute-NOCs, TrustedRootCertificates list validation [DUT-Server]</t>
         </is>
       </c>
       <c r="D454" s="3" t="inlineStr">
         <is>
-          <t>TC-CNET-1.3</t>
+          <t>TC-OPCREDS-3.1</t>
         </is>
       </c>
       <c r="E454" s="2" t="inlineStr">
@@ -11802,17 +11802,17 @@
       </c>
       <c r="B455" s="3" t="inlineStr">
         <is>
-          <t>Network Commissioning Test Plan</t>
+          <t>Node Operational Credentials Test Plan</t>
         </is>
       </c>
       <c r="C455" s="3" t="inlineStr">
         <is>
-          <t>[TC-CNET-4.2] [Thread] Verification for attributes check [DUT-Server]</t>
+          <t>[TC-OPCREDS-3.2] Attribute-CurrentFabricIndex validation [DUT-Server]</t>
         </is>
       </c>
       <c r="D455" s="3" t="inlineStr">
         <is>
-          <t>TC-CNET-4.2</t>
+          <t>TC-OPCREDS-3.2</t>
         </is>
       </c>
       <c r="E455" s="2" t="inlineStr">
@@ -11827,17 +11827,17 @@
       </c>
       <c r="B456" s="3" t="inlineStr">
         <is>
-          <t>Network Commissioning Test Plan</t>
+          <t>Node Operational Credentials Test Plan</t>
         </is>
       </c>
       <c r="C456" s="3" t="inlineStr">
         <is>
-          <t>[TC-CNET-4.3] [Ethernet] Verification for attributes check [DUT-Server]</t>
+          <t>[TC-OPCREDS-3.4] UpdateNOC-Error Condition [DUT-Server]</t>
         </is>
       </c>
       <c r="D456" s="3" t="inlineStr">
         <is>
-          <t>TC-CNET-4.3</t>
+          <t>TC-OPCREDS-3.4</t>
         </is>
       </c>
       <c r="E456" s="2" t="inlineStr">
@@ -11852,17 +11852,17 @@
       </c>
       <c r="B457" s="3" t="inlineStr">
         <is>
-          <t>Network Commissioning Test Plan</t>
+          <t>Node Operational Credentials Test Plan</t>
         </is>
       </c>
       <c r="C457" s="3" t="inlineStr">
         <is>
-          <t>[TC-CNET-4.4] [Wi-Fi] Verification for ScanNetworks command [DUT-Server]</t>
+          <t>[TC-OPCREDS-3.5] NOC Check for UpdateNOC [DUT-Server]</t>
         </is>
       </c>
       <c r="D457" s="3" t="inlineStr">
         <is>
-          <t>TC-CNET-4.4</t>
+          <t>TC-OPCREDS-3.5</t>
         </is>
       </c>
       <c r="E457" s="2" t="inlineStr">
@@ -11877,17 +11877,17 @@
       </c>
       <c r="B458" s="3" t="inlineStr">
         <is>
-          <t>Network Commissioning Test Plan</t>
+          <t>Node Operational Credentials Test Plan</t>
         </is>
       </c>
       <c r="C458" s="3" t="inlineStr">
         <is>
-          <t>[TC-CNET-4.5] [Wi-Fi] FAILSAFE_REQUIRED message Validation [DUT-Server]</t>
+          <t>[TC-OPCREDS-3.6] Last Fabric removal validation [DUT-Server]</t>
         </is>
       </c>
       <c r="D458" s="3" t="inlineStr">
         <is>
-          <t>TC-CNET-4.5</t>
+          <t>TC-OPCREDS-3.6</t>
         </is>
       </c>
       <c r="E458" s="2" t="inlineStr">
@@ -11902,17 +11902,17 @@
       </c>
       <c r="B459" s="3" t="inlineStr">
         <is>
-          <t>Network Commissioning Test Plan</t>
+          <t>Node Operational Credentials Test Plan</t>
         </is>
       </c>
       <c r="C459" s="3" t="inlineStr">
         <is>
-          <t>[TC-CNET-4.6] [Thread] FAILSAFE_REQUIRED message Validation [DUT-Server]</t>
+          <t>[TC-OPCREDS-3.7] Add Second Fabric over CASE [DUT-Server]</t>
         </is>
       </c>
       <c r="D459" s="3" t="inlineStr">
         <is>
-          <t>TC-CNET-4.6</t>
+          <t>TC-OPCREDS-3.7</t>
         </is>
       </c>
       <c r="E459" s="2" t="inlineStr">
@@ -11927,17 +11927,17 @@
       </c>
       <c r="B460" s="3" t="inlineStr">
         <is>
-          <t>Network Commissioning Test Plan</t>
+          <t>Node Operational Credentials Test Plan</t>
         </is>
       </c>
       <c r="C460" s="3" t="inlineStr">
         <is>
-          <t>[TC-CNET-4.9] [Wi-Fi] Verification for RemoveNetwork Command [DUT-Server]</t>
+          <t>[TC-OPCREDS-3.3] Attribute-NOCs, Commands [DUT-Client]</t>
         </is>
       </c>
       <c r="D460" s="3" t="inlineStr">
         <is>
-          <t>TC-CNET-4.9</t>
+          <t>TC-OPCREDS-3.3</t>
         </is>
       </c>
       <c r="E460" s="2" t="inlineStr">
@@ -11957,12 +11957,12 @@
       </c>
       <c r="C461" s="3" t="inlineStr">
         <is>
-          <t>[TC-CNET-4.10] [Thread] Verification for RemoveNetwork Command [DUT-Server]</t>
+          <t>[TC-CNET-1.3] Global Attributes with DUT as Server</t>
         </is>
       </c>
       <c r="D461" s="3" t="inlineStr">
         <is>
-          <t>TC-CNET-4.10</t>
+          <t>TC-CNET-1.3</t>
         </is>
       </c>
       <c r="E461" s="2" t="inlineStr">
@@ -11982,12 +11982,12 @@
       </c>
       <c r="C462" s="3" t="inlineStr">
         <is>
-          <t>[TC-CNET-4.11] [Wi-Fi] Verification for ConnectNetwork Command [DUT-Server]</t>
+          <t>[TC-CNET-4.2] [Thread] Verification for attributes check [DUT-Server]</t>
         </is>
       </c>
       <c r="D462" s="3" t="inlineStr">
         <is>
-          <t>TC-CNET-4.11</t>
+          <t>TC-CNET-4.2</t>
         </is>
       </c>
       <c r="E462" s="2" t="inlineStr">
@@ -12007,12 +12007,12 @@
       </c>
       <c r="C463" s="3" t="inlineStr">
         <is>
-          <t>[TC-CNET-4.12] [Thread] Verification for ConnectNetwork Command [DUT-Server]</t>
+          <t>[TC-CNET-4.3] [Ethernet] Verification for attributes check [DUT-Server]</t>
         </is>
       </c>
       <c r="D463" s="3" t="inlineStr">
         <is>
-          <t>TC-CNET-4.12</t>
+          <t>TC-CNET-4.3</t>
         </is>
       </c>
       <c r="E463" s="2" t="inlineStr">
@@ -12032,12 +12032,12 @@
       </c>
       <c r="C464" s="3" t="inlineStr">
         <is>
-          <t>[TC-CNET-4.13] [Wi-Fi] Verification for ReorderNetwork command [DUT-Server]</t>
+          <t>[TC-CNET-4.4] [Wi-Fi] Verification for ScanNetworks command [DUT-Server]</t>
         </is>
       </c>
       <c r="D464" s="3" t="inlineStr">
         <is>
-          <t>TC-CNET-4.13</t>
+          <t>TC-CNET-4.4</t>
         </is>
       </c>
       <c r="E464" s="2" t="inlineStr">
@@ -12057,12 +12057,12 @@
       </c>
       <c r="C465" s="3" t="inlineStr">
         <is>
-          <t>[TC-CNET-4.14] [Thread] Verification for ReorderNetwork command [DUT-Server]</t>
+          <t>[TC-CNET-4.5] [Wi-Fi] FAILSAFE_REQUIRED message Validation [DUT-Server]</t>
         </is>
       </c>
       <c r="D465" s="3" t="inlineStr">
         <is>
-          <t>TC-CNET-4.14</t>
+          <t>TC-CNET-4.5</t>
         </is>
       </c>
       <c r="E465" s="2" t="inlineStr">
@@ -12082,12 +12082,12 @@
       </c>
       <c r="C466" s="3" t="inlineStr">
         <is>
-          <t>[TC-CNET-4.15] [Wi-Fi] NetworkIDNotFound returned in LastNetworkingStatus field validation [DUT-Server]</t>
+          <t>[TC-CNET-4.6] [Thread] FAILSAFE_REQUIRED message Validation [DUT-Server]</t>
         </is>
       </c>
       <c r="D466" s="3" t="inlineStr">
         <is>
-          <t>TC-CNET-4.15</t>
+          <t>TC-CNET-4.6</t>
         </is>
       </c>
       <c r="E466" s="2" t="inlineStr">
@@ -12107,12 +12107,12 @@
       </c>
       <c r="C467" s="3" t="inlineStr">
         <is>
-          <t>[TC-CNET-4.16] [Thread] NetworkIDNotFound returned in LastNetworkingStatus field validation [DUT-Server]</t>
+          <t>[TC-CNET-4.9] [Wi-Fi] Verification for RemoveNetwork Command [DUT-Server]</t>
         </is>
       </c>
       <c r="D467" s="3" t="inlineStr">
         <is>
-          <t>TC-CNET-4.16</t>
+          <t>TC-CNET-4.9</t>
         </is>
       </c>
       <c r="E467" s="2" t="inlineStr">
@@ -12132,12 +12132,12 @@
       </c>
       <c r="C468" s="3" t="inlineStr">
         <is>
-          <t>[TC-CNET-4.22] [Thread] Verification for ScanNetworks command [DUT-Server]</t>
+          <t>[TC-CNET-4.10] [Thread] Verification for RemoveNetwork Command [DUT-Server]</t>
         </is>
       </c>
       <c r="D468" s="3" t="inlineStr">
         <is>
-          <t>TC-CNET-4.22</t>
+          <t>TC-CNET-4.10</t>
         </is>
       </c>
       <c r="E468" s="2" t="inlineStr">
@@ -12157,12 +12157,12 @@
       </c>
       <c r="C469" s="3" t="inlineStr">
         <is>
-          <t>[TC-CNET-4.20] [Wi-Fi] Verification for commands check  [DUT-Client]</t>
+          <t>[TC-CNET-4.11] [Wi-Fi] Verification for ConnectNetwork Command [DUT-Server]</t>
         </is>
       </c>
       <c r="D469" s="3" t="inlineStr">
         <is>
-          <t>TC-CNET-4.20</t>
+          <t>TC-CNET-4.11</t>
         </is>
       </c>
       <c r="E469" s="2" t="inlineStr">
@@ -12182,12 +12182,12 @@
       </c>
       <c r="C470" s="3" t="inlineStr">
         <is>
-          <t>[TC-CNET-4.21] [Thread] Verification for commands check  [DUT-Client]</t>
+          <t>[TC-CNET-4.12] [Thread] Verification for ConnectNetwork Command [DUT-Server]</t>
         </is>
       </c>
       <c r="D470" s="3" t="inlineStr">
         <is>
-          <t>TC-CNET-4.21</t>
+          <t>TC-CNET-4.12</t>
         </is>
       </c>
       <c r="E470" s="2" t="inlineStr">
@@ -12202,17 +12202,17 @@
       </c>
       <c r="B471" s="3" t="inlineStr">
         <is>
-          <t>Secure Channel Test Plan</t>
+          <t>Network Commissioning Test Plan</t>
         </is>
       </c>
       <c r="C471" s="3" t="inlineStr">
         <is>
-          <t>[TC-SC-1.1] MRP Max Message Size - REMOVED</t>
+          <t>[TC-CNET-4.13] [Wi-Fi] Verification for ReorderNetwork command [DUT-Server]</t>
         </is>
       </c>
       <c r="D471" s="3" t="inlineStr">
         <is>
-          <t>TC-SC-1.1</t>
+          <t>TC-CNET-4.13</t>
         </is>
       </c>
       <c r="E471" s="2" t="inlineStr">
@@ -12227,17 +12227,17 @@
       </c>
       <c r="B472" s="3" t="inlineStr">
         <is>
-          <t>Secure Channel Test Plan</t>
+          <t>Network Commissioning Test Plan</t>
         </is>
       </c>
       <c r="C472" s="3" t="inlineStr">
         <is>
-          <t>[TC-SC-1.2] MRP Message Flows - REMOVED</t>
+          <t>[TC-CNET-4.14] [Thread] Verification for ReorderNetwork command [DUT-Server]</t>
         </is>
       </c>
       <c r="D472" s="3" t="inlineStr">
         <is>
-          <t>TC-SC-1.2</t>
+          <t>TC-CNET-4.14</t>
         </is>
       </c>
       <c r="E472" s="2" t="inlineStr">
@@ -12252,17 +12252,17 @@
       </c>
       <c r="B473" s="3" t="inlineStr">
         <is>
-          <t>Secure Channel Test Plan</t>
+          <t>Network Commissioning Test Plan</t>
         </is>
       </c>
       <c r="C473" s="3" t="inlineStr">
         <is>
-          <t>[TC-SC-1.3] MRP Retransmissions - REMOVED</t>
+          <t>[TC-CNET-4.15] [Wi-Fi] NetworkIDNotFound returned in LastNetworkingStatus field validation [DUT-Server]</t>
         </is>
       </c>
       <c r="D473" s="3" t="inlineStr">
         <is>
-          <t>TC-SC-1.3</t>
+          <t>TC-CNET-4.15</t>
         </is>
       </c>
       <c r="E473" s="2" t="inlineStr">
@@ -12277,17 +12277,17 @@
       </c>
       <c r="B474" s="3" t="inlineStr">
         <is>
-          <t>Secure Channel Test Plan</t>
+          <t>Network Commissioning Test Plan</t>
         </is>
       </c>
       <c r="C474" s="3" t="inlineStr">
         <is>
-          <t>[TC-SC-1.4] MRP message counter and duplicate messaging - REMOVED</t>
+          <t>[TC-CNET-4.16] [Thread] NetworkIDNotFound returned in LastNetworkingStatus field validation [DUT-Server]</t>
         </is>
       </c>
       <c r="D474" s="3" t="inlineStr">
         <is>
-          <t>TC-SC-1.4</t>
+          <t>TC-CNET-4.16</t>
         </is>
       </c>
       <c r="E474" s="2" t="inlineStr">
@@ -12302,17 +12302,17 @@
       </c>
       <c r="B475" s="3" t="inlineStr">
         <is>
-          <t>Secure Channel Test Plan</t>
+          <t>Network Commissioning Test Plan</t>
         </is>
       </c>
       <c r="C475" s="3" t="inlineStr">
         <is>
-          <t>[TC-SC-2.1] Session Establishment - Passcode Authenticated Session Establishment (PASE) - REMOVED</t>
+          <t>[TC-CNET-4.22] [Thread] Verification for ScanNetworks command [DUT-Server]</t>
         </is>
       </c>
       <c r="D475" s="3" t="inlineStr">
         <is>
-          <t>TC-SC-2.1</t>
+          <t>TC-CNET-4.22</t>
         </is>
       </c>
       <c r="E475" s="2" t="inlineStr">
@@ -12327,17 +12327,17 @@
       </c>
       <c r="B476" s="3" t="inlineStr">
         <is>
-          <t>Secure Channel Test Plan</t>
+          <t>Network Commissioning Test Plan</t>
         </is>
       </c>
       <c r="C476" s="3" t="inlineStr">
         <is>
-          <t>[TC-SC-2.2] Bidirectional Communication - Passcode Authenticated Session Establishment (PASE) - REMOVED</t>
+          <t>[TC-CNET-4.20] [Wi-Fi] Verification for commands check  [DUT-Client]</t>
         </is>
       </c>
       <c r="D476" s="3" t="inlineStr">
         <is>
-          <t>TC-SC-2.2</t>
+          <t>TC-CNET-4.20</t>
         </is>
       </c>
       <c r="E476" s="2" t="inlineStr">
@@ -12352,17 +12352,17 @@
       </c>
       <c r="B477" s="3" t="inlineStr">
         <is>
-          <t>Secure Channel Test Plan</t>
+          <t>Network Commissioning Test Plan</t>
         </is>
       </c>
       <c r="C477" s="3" t="inlineStr">
         <is>
-          <t>[TC-SC-2.3] PASE Error Handling [DUT_Responder/Commissionee] - REMOVED</t>
+          <t>[TC-CNET-4.21] [Thread] Verification for commands check  [DUT-Client]</t>
         </is>
       </c>
       <c r="D477" s="3" t="inlineStr">
         <is>
-          <t>TC-SC-2.3</t>
+          <t>TC-CNET-4.21</t>
         </is>
       </c>
       <c r="E477" s="2" t="inlineStr">
@@ -12382,12 +12382,12 @@
       </c>
       <c r="C478" s="3" t="inlineStr">
         <is>
-          <t>[TC-SC-2.4] PASE Error Handling [DUT_Initiator/Commissioner] - REMOVED</t>
+          <t>[TC-SC-1.1] MRP Max Message Size - REMOVED</t>
         </is>
       </c>
       <c r="D478" s="3" t="inlineStr">
         <is>
-          <t>TC-SC-2.4</t>
+          <t>TC-SC-1.1</t>
         </is>
       </c>
       <c r="E478" s="2" t="inlineStr">
@@ -12407,12 +12407,12 @@
       </c>
       <c r="C479" s="3" t="inlineStr">
         <is>
-          <t>[TC-SC-3.1] Session Establishment - REMOVED</t>
+          <t>[TC-SC-1.2] MRP Message Flows - REMOVED</t>
         </is>
       </c>
       <c r="D479" s="3" t="inlineStr">
         <is>
-          <t>TC-SC-3.1</t>
+          <t>TC-SC-1.2</t>
         </is>
       </c>
       <c r="E479" s="2" t="inlineStr">
@@ -12432,12 +12432,12 @@
       </c>
       <c r="C480" s="3" t="inlineStr">
         <is>
-          <t>[TC-SC-3.2] CASE Session Resumption [DUT_Responder]</t>
+          <t>[TC-SC-1.3] MRP Retransmissions - REMOVED</t>
         </is>
       </c>
       <c r="D480" s="3" t="inlineStr">
         <is>
-          <t>TC-SC-3.2</t>
+          <t>TC-SC-1.3</t>
         </is>
       </c>
       <c r="E480" s="2" t="inlineStr">
@@ -12457,12 +12457,12 @@
       </c>
       <c r="C481" s="3" t="inlineStr">
         <is>
-          <t>[TC-SC-3.3] CASE Session Resumption [DUT_Initiator] - REMOVED</t>
+          <t>[TC-SC-1.4] MRP message counter and duplicate messaging - REMOVED</t>
         </is>
       </c>
       <c r="D481" s="3" t="inlineStr">
         <is>
-          <t>TC-SC-3.3</t>
+          <t>TC-SC-1.4</t>
         </is>
       </c>
       <c r="E481" s="2" t="inlineStr">
@@ -12482,12 +12482,12 @@
       </c>
       <c r="C482" s="3" t="inlineStr">
         <is>
-          <t>[TC-SC-3.4] CASE Error Handling [DUT_Responder] - REMOVED</t>
+          <t>[TC-SC-2.1] Session Establishment - Passcode Authenticated Session Establishment (PASE) - REMOVED</t>
         </is>
       </c>
       <c r="D482" s="3" t="inlineStr">
         <is>
-          <t>TC-SC-3.4</t>
+          <t>TC-SC-2.1</t>
         </is>
       </c>
       <c r="E482" s="2" t="inlineStr">
@@ -12507,12 +12507,12 @@
       </c>
       <c r="C483" s="3" t="inlineStr">
         <is>
-          <t>[TC-SC-3.5] CASE Error Handling [DUT_Initiator] - REMOVED</t>
+          <t>[TC-SC-2.2] Bidirectional Communication - Passcode Authenticated Session Establishment (PASE) - REMOVED</t>
         </is>
       </c>
       <c r="D483" s="3" t="inlineStr">
         <is>
-          <t>TC-SC-3.5</t>
+          <t>TC-SC-2.2</t>
         </is>
       </c>
       <c r="E483" s="2" t="inlineStr">
@@ -12532,12 +12532,12 @@
       </c>
       <c r="C484" s="3" t="inlineStr">
         <is>
-          <t>[TC-SC-3.6] CASE Resource validation</t>
+          <t>[TC-SC-2.3] PASE Error Handling [DUT_Responder/Commissionee] - REMOVED</t>
         </is>
       </c>
       <c r="D484" s="3" t="inlineStr">
         <is>
-          <t>TC-SC-3.6</t>
+          <t>TC-SC-2.3</t>
         </is>
       </c>
       <c r="E484" s="2" t="inlineStr">
@@ -12557,12 +12557,12 @@
       </c>
       <c r="C485" s="3" t="inlineStr">
         <is>
-          <t>[TC-SC-4.1] Commissionable Node Discovery [DUT as Commissionee]</t>
+          <t>[TC-SC-2.4] PASE Error Handling [DUT_Initiator/Commissioner] - REMOVED</t>
         </is>
       </c>
       <c r="D485" s="3" t="inlineStr">
         <is>
-          <t>TC-SC-4.1</t>
+          <t>TC-SC-2.4</t>
         </is>
       </c>
       <c r="E485" s="2" t="inlineStr">
@@ -12582,12 +12582,12 @@
       </c>
       <c r="C486" s="3" t="inlineStr">
         <is>
-          <t>[TC-SC-4.2] Discovery [DUT as Commissioner]</t>
+          <t>[TC-SC-3.1] Session Establishment - REMOVED</t>
         </is>
       </c>
       <c r="D486" s="3" t="inlineStr">
         <is>
-          <t>TC-SC-4.2</t>
+          <t>TC-SC-3.1</t>
         </is>
       </c>
       <c r="E486" s="2" t="inlineStr">
@@ -12607,12 +12607,12 @@
       </c>
       <c r="C487" s="3" t="inlineStr">
         <is>
-          <t>[TC-SC-4.3] Discovery [DUT as Commissionee]</t>
+          <t>[TC-SC-3.2] CASE Session Resumption [DUT_Responder]</t>
         </is>
       </c>
       <c r="D487" s="3" t="inlineStr">
         <is>
-          <t>TC-SC-4.3</t>
+          <t>TC-SC-3.2</t>
         </is>
       </c>
       <c r="E487" s="2" t="inlineStr">
@@ -12632,12 +12632,12 @@
       </c>
       <c r="C488" s="3" t="inlineStr">
         <is>
-          <t>[TC-SC-4.4] Discovery [DUT as Controller]</t>
+          <t>[TC-SC-3.3] CASE Session Resumption [DUT_Initiator] - REMOVED</t>
         </is>
       </c>
       <c r="D488" s="3" t="inlineStr">
         <is>
-          <t>TC-SC-4.4</t>
+          <t>TC-SC-3.3</t>
         </is>
       </c>
       <c r="E488" s="2" t="inlineStr">
@@ -12657,12 +12657,12 @@
       </c>
       <c r="C489" s="3" t="inlineStr">
         <is>
-          <t>[TC-SC-4.5] Discovery [DUT as Commissionee][Thread] - REMOVED</t>
+          <t>[TC-SC-3.4] CASE Error Handling [DUT_Responder] - REMOVED</t>
         </is>
       </c>
       <c r="D489" s="3" t="inlineStr">
         <is>
-          <t>TC-SC-4.5</t>
+          <t>TC-SC-3.4</t>
         </is>
       </c>
       <c r="E489" s="2" t="inlineStr">
@@ -12682,12 +12682,12 @@
       </c>
       <c r="C490" s="3" t="inlineStr">
         <is>
-          <t>[TC-SC-4.6] Commissioner Discovery [DUT as Commissioner]</t>
+          <t>[TC-SC-3.5] CASE Error Handling [DUT_Initiator] - REMOVED</t>
         </is>
       </c>
       <c r="D490" s="3" t="inlineStr">
         <is>
-          <t>TC-SC-4.6</t>
+          <t>TC-SC-3.5</t>
         </is>
       </c>
       <c r="E490" s="2" t="inlineStr">
@@ -12707,12 +12707,12 @@
       </c>
       <c r="C491" s="3" t="inlineStr">
         <is>
-          <t>[TC-SC-4.7] Commissioner Discovery [DUT as Commissionee]</t>
+          <t>[TC-SC-3.6] CASE Resource validation</t>
         </is>
       </c>
       <c r="D491" s="3" t="inlineStr">
         <is>
-          <t>TC-SC-4.7</t>
+          <t>TC-SC-3.6</t>
         </is>
       </c>
       <c r="E491" s="2" t="inlineStr">
@@ -12732,12 +12732,12 @@
       </c>
       <c r="C492" s="3" t="inlineStr">
         <is>
-          <t>[TC-SC-4.8] Compressed Fabric ID remains the same for Nodes commissioned to the same fabric [DUT as Commissioner]</t>
+          <t>[TC-SC-4.1] Commissionable Node Discovery [DUT as Commissionee]</t>
         </is>
       </c>
       <c r="D492" s="3" t="inlineStr">
         <is>
-          <t>TC-SC-4.8</t>
+          <t>TC-SC-4.1</t>
         </is>
       </c>
       <c r="E492" s="2" t="inlineStr">
@@ -12757,12 +12757,12 @@
       </c>
       <c r="C493" s="3" t="inlineStr">
         <is>
-          <t>[TC-SC-4.9] Operational Discovery - RIO support [DUT as Commissionee]</t>
+          <t>[TC-SC-4.2] Discovery [DUT as Commissioner]</t>
         </is>
       </c>
       <c r="D493" s="3" t="inlineStr">
         <is>
-          <t>TC-SC-4.9</t>
+          <t>TC-SC-4.2</t>
         </is>
       </c>
       <c r="E493" s="2" t="inlineStr">
@@ -12782,12 +12782,12 @@
       </c>
       <c r="C494" s="3" t="inlineStr">
         <is>
-          <t>[TC-SC-4.10] Operational Discovery - SIT ICD Node [DUT as Commissionee]</t>
+          <t>[TC-SC-4.3] Discovery [DUT as Commissionee]</t>
         </is>
       </c>
       <c r="D494" s="3" t="inlineStr">
         <is>
-          <t>TC-SC-4.10</t>
+          <t>TC-SC-4.3</t>
         </is>
       </c>
       <c r="E494" s="2" t="inlineStr">
@@ -12802,17 +12802,17 @@
       </c>
       <c r="B495" s="3" t="inlineStr">
         <is>
-          <t>Group Communication</t>
+          <t>Secure Channel Test Plan</t>
         </is>
       </c>
       <c r="C495" s="3" t="inlineStr">
         <is>
-          <t>[TC-GRPKEY-1.1] Global Attributes with DUT as Server</t>
+          <t>[TC-SC-4.4] Discovery [DUT as Controller]</t>
         </is>
       </c>
       <c r="D495" s="3" t="inlineStr">
         <is>
-          <t>TC-GRPKEY-1.1</t>
+          <t>TC-SC-4.4</t>
         </is>
       </c>
       <c r="E495" s="2" t="inlineStr">
@@ -12827,17 +12827,17 @@
       </c>
       <c r="B496" s="3" t="inlineStr">
         <is>
-          <t>Group Communication</t>
+          <t>Secure Channel Test Plan</t>
         </is>
       </c>
       <c r="C496" s="3" t="inlineStr">
         <is>
-          <t>[TC-GRPKEY-2.1] Attributes [DUT-Server]</t>
+          <t>[TC-SC-4.5] Discovery [DUT as Commissionee][Thread] - REMOVED</t>
         </is>
       </c>
       <c r="D496" s="3" t="inlineStr">
         <is>
-          <t>TC-GRPKEY-2.1</t>
+          <t>TC-SC-4.5</t>
         </is>
       </c>
       <c r="E496" s="2" t="inlineStr">
@@ -12852,17 +12852,17 @@
       </c>
       <c r="B497" s="3" t="inlineStr">
         <is>
-          <t>Group Communication</t>
+          <t>Secure Channel Test Plan</t>
         </is>
       </c>
       <c r="C497" s="3" t="inlineStr">
         <is>
-          <t>[TC-GRPKEY-2.2] Primary functionality with DUT as Server</t>
+          <t>[TC-SC-4.6] Commissioner Discovery [DUT as Commissioner]</t>
         </is>
       </c>
       <c r="D497" s="3" t="inlineStr">
         <is>
-          <t>TC-GRPKEY-2.2</t>
+          <t>TC-SC-4.6</t>
         </is>
       </c>
       <c r="E497" s="2" t="inlineStr">
@@ -12877,17 +12877,17 @@
       </c>
       <c r="B498" s="3" t="inlineStr">
         <is>
-          <t>Group Communication</t>
+          <t>Secure Channel Test Plan</t>
         </is>
       </c>
       <c r="C498" s="3" t="inlineStr">
         <is>
-          <t>[TC-SC-5.1] Adding member to a group - TH as Admin and DUT as Group Member</t>
+          <t>[TC-SC-4.7] Commissioner Discovery [DUT as Commissionee]</t>
         </is>
       </c>
       <c r="D498" s="3" t="inlineStr">
         <is>
-          <t>TC-SC-5.1</t>
+          <t>TC-SC-4.7</t>
         </is>
       </c>
       <c r="E498" s="2" t="inlineStr">
@@ -12902,17 +12902,17 @@
       </c>
       <c r="B499" s="3" t="inlineStr">
         <is>
-          <t>Group Communication</t>
+          <t>Secure Channel Test Plan</t>
         </is>
       </c>
       <c r="C499" s="3" t="inlineStr">
         <is>
-          <t>[TC-SC-5.2] Receiving a group message - TH to DUT</t>
+          <t>[TC-SC-4.8] Compressed Fabric ID remains the same for Nodes commissioned to the same fabric [DUT as Commissioner]</t>
         </is>
       </c>
       <c r="D499" s="3" t="inlineStr">
         <is>
-          <t>TC-SC-5.2</t>
+          <t>TC-SC-4.8</t>
         </is>
       </c>
       <c r="E499" s="2" t="inlineStr">
@@ -12927,17 +12927,17 @@
       </c>
       <c r="B500" s="3" t="inlineStr">
         <is>
-          <t>Group Communication</t>
+          <t>Secure Channel Test Plan</t>
         </is>
       </c>
       <c r="C500" s="3" t="inlineStr">
         <is>
-          <t>[TC-SC-5.3] Sending a group message - DUT to TH</t>
+          <t>[TC-SC-4.9] Operational Discovery - RIO support [DUT as Commissionee]</t>
         </is>
       </c>
       <c r="D500" s="3" t="inlineStr">
         <is>
-          <t>TC-SC-5.3</t>
+          <t>TC-SC-4.9</t>
         </is>
       </c>
       <c r="E500" s="2" t="inlineStr">
@@ -12952,17 +12952,17 @@
       </c>
       <c r="B501" s="3" t="inlineStr">
         <is>
-          <t>Group Communication</t>
+          <t>Secure Channel Test Plan</t>
         </is>
       </c>
       <c r="C501" s="3" t="inlineStr">
         <is>
-          <t>[TC-GRPKEY-5.4] Verification for KeySetReadResponse Command for CacheAndSync</t>
+          <t>[TC-SC-4.10] Operational Discovery - SIT ICD Node [DUT as Commissionee]</t>
         </is>
       </c>
       <c r="D501" s="3" t="inlineStr">
         <is>
-          <t>TC-GRPKEY-5.4</t>
+          <t>TC-SC-4.10</t>
         </is>
       </c>
       <c r="E501" s="2" t="inlineStr">
@@ -12982,12 +12982,12 @@
       </c>
       <c r="C502" s="3" t="inlineStr">
         <is>
-          <t>[TC-SC-6.1] Adding member to a group - DUT as Admin and TH as Group Member [DUT-Client]</t>
+          <t>[TC-GRPKEY-1.1] Global Attributes with DUT as Server</t>
         </is>
       </c>
       <c r="D502" s="3" t="inlineStr">
         <is>
-          <t>TC-SC-6.1</t>
+          <t>TC-GRPKEY-1.1</t>
         </is>
       </c>
       <c r="E502" s="2" t="inlineStr">
@@ -13002,17 +13002,17 @@
       </c>
       <c r="B503" s="3" t="inlineStr">
         <is>
-          <t>Device Attestation Test Plan</t>
+          <t>Group Communication</t>
         </is>
       </c>
       <c r="C503" s="3" t="inlineStr">
         <is>
-          <t>[TC-DA-1.1] The NOC SHALL be wiped on Factory Reset [DUT - Commissionee]</t>
+          <t>[TC-GRPKEY-2.1] Attributes [DUT-Server]</t>
         </is>
       </c>
       <c r="D503" s="3" t="inlineStr">
         <is>
-          <t>TC-DA-1.1</t>
+          <t>TC-GRPKEY-2.1</t>
         </is>
       </c>
       <c r="E503" s="2" t="inlineStr">
@@ -13027,17 +13027,17 @@
       </c>
       <c r="B504" s="3" t="inlineStr">
         <is>
-          <t>Device Attestation Test Plan</t>
+          <t>Group Communication</t>
         </is>
       </c>
       <c r="C504" s="3" t="inlineStr">
         <is>
-          <t>[TC-DA-1.2] Device Attestation Request Validation [DUT - Commissionee]</t>
+          <t>[TC-GRPKEY-2.2] Primary functionality with DUT as Server</t>
         </is>
       </c>
       <c r="D504" s="3" t="inlineStr">
         <is>
-          <t>TC-DA-1.2</t>
+          <t>TC-GRPKEY-2.2</t>
         </is>
       </c>
       <c r="E504" s="2" t="inlineStr">
@@ -13052,17 +13052,17 @@
       </c>
       <c r="B505" s="3" t="inlineStr">
         <is>
-          <t>Device Attestation Test Plan</t>
+          <t>Group Communication</t>
         </is>
       </c>
       <c r="C505" s="3" t="inlineStr">
         <is>
-          <t>[TC-DA-1.3] Device Attestation Request Validation [DUT - Commissioner]</t>
+          <t>[TC-SC-5.1] Adding member to a group - TH as Admin and DUT as Group Member</t>
         </is>
       </c>
       <c r="D505" s="3" t="inlineStr">
         <is>
-          <t>TC-DA-1.3</t>
+          <t>TC-SC-5.1</t>
         </is>
       </c>
       <c r="E505" s="2" t="inlineStr">
@@ -13077,17 +13077,17 @@
       </c>
       <c r="B506" s="3" t="inlineStr">
         <is>
-          <t>Device Attestation Test Plan</t>
+          <t>Group Communication</t>
         </is>
       </c>
       <c r="C506" s="3" t="inlineStr">
         <is>
-          <t>[TC-DA-1.4] Device Attestation Request Validation-Error Scenario [DUT-Commissioner]</t>
+          <t>[TC-SC-5.2] Receiving a group message - TH to DUT</t>
         </is>
       </c>
       <c r="D506" s="3" t="inlineStr">
         <is>
-          <t>TC-DA-1.4</t>
+          <t>TC-SC-5.2</t>
         </is>
       </c>
       <c r="E506" s="2" t="inlineStr">
@@ -13102,17 +13102,17 @@
       </c>
       <c r="B507" s="3" t="inlineStr">
         <is>
-          <t>Device Attestation Test Plan</t>
+          <t>Group Communication</t>
         </is>
       </c>
       <c r="C507" s="3" t="inlineStr">
         <is>
-          <t>[TC-DA-1.5] NOCSR Procedure Validation [DUT - Commissionee]</t>
+          <t>[TC-SC-5.3] Sending a group message - DUT to TH</t>
         </is>
       </c>
       <c r="D507" s="3" t="inlineStr">
         <is>
-          <t>TC-DA-1.5</t>
+          <t>TC-SC-5.3</t>
         </is>
       </c>
       <c r="E507" s="2" t="inlineStr">
@@ -13127,17 +13127,17 @@
       </c>
       <c r="B508" s="3" t="inlineStr">
         <is>
-          <t>Device Attestation Test Plan</t>
+          <t>Group Communication</t>
         </is>
       </c>
       <c r="C508" s="3" t="inlineStr">
         <is>
-          <t>[TC-DA-1.6] NOCSR Procedure Validation [DUT - Commissioner]</t>
+          <t>[TC-GRPKEY-5.4] Verification for KeySetReadResponse Command for CacheAndSync</t>
         </is>
       </c>
       <c r="D508" s="3" t="inlineStr">
         <is>
-          <t>TC-DA-1.6</t>
+          <t>TC-GRPKEY-5.4</t>
         </is>
       </c>
       <c r="E508" s="2" t="inlineStr">
@@ -13152,17 +13152,17 @@
       </c>
       <c r="B509" s="3" t="inlineStr">
         <is>
-          <t>Device Attestation Test Plan</t>
+          <t>Group Communication</t>
         </is>
       </c>
       <c r="C509" s="3" t="inlineStr">
         <is>
-          <t>[TC-DA-1.7] Validate CertificateChainRequest [DUT-Commissionee]</t>
+          <t>[TC-SC-6.1] Adding member to a group - DUT as Admin and TH as Group Member [DUT-Client]</t>
         </is>
       </c>
       <c r="D509" s="3" t="inlineStr">
         <is>
-          <t>TC-DA-1.7</t>
+          <t>TC-SC-6.1</t>
         </is>
       </c>
       <c r="E509" s="2" t="inlineStr">
@@ -13182,12 +13182,12 @@
       </c>
       <c r="C510" s="3" t="inlineStr">
         <is>
-          <t>[TC-DA-1.8] Device Attestation Request Validation-Success Scenario [DUT-Commissioner]</t>
+          <t>[TC-DA-1.1] The NOC SHALL be wiped on Factory Reset [DUT - Commissionee]</t>
         </is>
       </c>
       <c r="D510" s="3" t="inlineStr">
         <is>
-          <t>TC-DA-1.8</t>
+          <t>TC-DA-1.1</t>
         </is>
       </c>
       <c r="E510" s="2" t="inlineStr">
@@ -13202,17 +13202,17 @@
       </c>
       <c r="B511" s="3" t="inlineStr">
         <is>
-          <t>Interaction Data Model Test Plan</t>
+          <t>Device Attestation Test Plan</t>
         </is>
       </c>
       <c r="C511" s="3" t="inlineStr">
         <is>
-          <t>[TC-IDM-1.1] Invoke Request Action from DUT to TH - [DUT as Client]</t>
+          <t>[TC-DA-1.2] Device Attestation Request Validation [DUT - Commissionee]</t>
         </is>
       </c>
       <c r="D511" s="3" t="inlineStr">
         <is>
-          <t>TC-IDM-1.1</t>
+          <t>TC-DA-1.2</t>
         </is>
       </c>
       <c r="E511" s="2" t="inlineStr">
@@ -13227,17 +13227,17 @@
       </c>
       <c r="B512" s="3" t="inlineStr">
         <is>
-          <t>Interaction Data Model Test Plan</t>
+          <t>Device Attestation Test Plan</t>
         </is>
       </c>
       <c r="C512" s="3" t="inlineStr">
         <is>
-          <t>[TC-IDM-1.2] Invoke Response Action from DUT to TH - [DUT as Server]</t>
+          <t>[TC-DA-1.3] Device Attestation Request Validation [DUT - Commissioner]</t>
         </is>
       </c>
       <c r="D512" s="3" t="inlineStr">
         <is>
-          <t>TC-IDM-1.2</t>
+          <t>TC-DA-1.3</t>
         </is>
       </c>
       <c r="E512" s="2" t="inlineStr">
@@ -13252,17 +13252,17 @@
       </c>
       <c r="B513" s="3" t="inlineStr">
         <is>
-          <t>Interaction Data Model Test Plan</t>
+          <t>Device Attestation Test Plan</t>
         </is>
       </c>
       <c r="C513" s="3" t="inlineStr">
         <is>
-          <t>[TC-IDM-2.1] Read Request Action from DUT to TH. [DUT as Client]</t>
+          <t>[TC-DA-1.4] Device Attestation Request Validation-Error Scenario [DUT-Commissioner]</t>
         </is>
       </c>
       <c r="D513" s="3" t="inlineStr">
         <is>
-          <t>TC-IDM-2.1</t>
+          <t>TC-DA-1.4</t>
         </is>
       </c>
       <c r="E513" s="2" t="inlineStr">
@@ -13277,17 +13277,17 @@
       </c>
       <c r="B514" s="3" t="inlineStr">
         <is>
-          <t>Interaction Data Model Test Plan</t>
+          <t>Device Attestation Test Plan</t>
         </is>
       </c>
       <c r="C514" s="3" t="inlineStr">
         <is>
-          <t>[TC-IDM-2.2] Report Data Action from DUT to TH. [DUT as Server]</t>
+          <t>[TC-DA-1.5] NOCSR Procedure Validation [DUT - Commissionee]</t>
         </is>
       </c>
       <c r="D514" s="3" t="inlineStr">
         <is>
-          <t>TC-IDM-2.2</t>
+          <t>TC-DA-1.5</t>
         </is>
       </c>
       <c r="E514" s="2" t="inlineStr">
@@ -13302,17 +13302,17 @@
       </c>
       <c r="B515" s="3" t="inlineStr">
         <is>
-          <t>Interaction Data Model Test Plan</t>
+          <t>Device Attestation Test Plan</t>
         </is>
       </c>
       <c r="C515" s="3" t="inlineStr">
         <is>
-          <t>[TC-IDM-3.1] Write Request Action from DUT to TH. [DUT as Client]</t>
+          <t>[TC-DA-1.6] NOCSR Procedure Validation [DUT - Commissioner]</t>
         </is>
       </c>
       <c r="D515" s="3" t="inlineStr">
         <is>
-          <t>TC-IDM-3.1</t>
+          <t>TC-DA-1.6</t>
         </is>
       </c>
       <c r="E515" s="2" t="inlineStr">
@@ -13327,17 +13327,17 @@
       </c>
       <c r="B516" s="3" t="inlineStr">
         <is>
-          <t>Interaction Data Model Test Plan</t>
+          <t>Device Attestation Test Plan</t>
         </is>
       </c>
       <c r="C516" s="3" t="inlineStr">
         <is>
-          <t>[TC-IDM-3.2] Write Response Action from DUT to TH. [DUT as Server]</t>
+          <t>[TC-DA-1.7] Validate CertificateChainRequest [DUT-Commissionee]</t>
         </is>
       </c>
       <c r="D516" s="3" t="inlineStr">
         <is>
-          <t>TC-IDM-3.2</t>
+          <t>TC-DA-1.7</t>
         </is>
       </c>
       <c r="E516" s="2" t="inlineStr">
@@ -13352,17 +13352,17 @@
       </c>
       <c r="B517" s="3" t="inlineStr">
         <is>
-          <t>Interaction Data Model Test Plan</t>
+          <t>Device Attestation Test Plan</t>
         </is>
       </c>
       <c r="C517" s="3" t="inlineStr">
         <is>
-          <t>[TC-IDM-4.1] SubscriptionRequestMessage from DUT test cases. [DUT as Client]</t>
+          <t>[TC-DA-1.8] Device Attestation Request Validation-Success Scenario [DUT-Commissioner]</t>
         </is>
       </c>
       <c r="D517" s="3" t="inlineStr">
         <is>
-          <t>TC-IDM-4.1</t>
+          <t>TC-DA-1.8</t>
         </is>
       </c>
       <c r="E517" s="2" t="inlineStr">
@@ -13382,12 +13382,12 @@
       </c>
       <c r="C518" s="3" t="inlineStr">
         <is>
-          <t>[TC-IDM-4.2] Subscription Response Messages from DUT Test Cases. [DUT as Server]</t>
+          <t>[TC-IDM-1.1] Invoke Request Action from DUT to TH - [DUT as Client]</t>
         </is>
       </c>
       <c r="D518" s="3" t="inlineStr">
         <is>
-          <t>TC-IDM-4.2</t>
+          <t>TC-IDM-1.1</t>
         </is>
       </c>
       <c r="E518" s="2" t="inlineStr">
@@ -13407,12 +13407,12 @@
       </c>
       <c r="C519" s="3" t="inlineStr">
         <is>
-          <t>[TC-IDM-4.3] Report Data Messages post Subscription Activation from DUT Test Cases. [DUT as Server]</t>
+          <t>[TC-IDM-1.2] Invoke Response Action from DUT to TH - [DUT as Server]</t>
         </is>
       </c>
       <c r="D519" s="3" t="inlineStr">
         <is>
-          <t>TC-IDM-4.3</t>
+          <t>TC-IDM-1.2</t>
         </is>
       </c>
       <c r="E519" s="2" t="inlineStr">
@@ -13432,12 +13432,12 @@
       </c>
       <c r="C520" s="3" t="inlineStr">
         <is>
-          <t>[TC-IDM-4.4] Persistent Subscription Test Cases. [DUT as Server]</t>
+          <t>[TC-IDM-2.1] Read Request Action from DUT to TH. [DUT as Client]</t>
         </is>
       </c>
       <c r="D520" s="3" t="inlineStr">
         <is>
-          <t>TC-IDM-4.4</t>
+          <t>TC-IDM-2.1</t>
         </is>
       </c>
       <c r="E520" s="2" t="inlineStr">
@@ -13457,12 +13457,12 @@
       </c>
       <c r="C521" s="3" t="inlineStr">
         <is>
-          <t>[TC-IDM-5.1] Timed Request Action from DUT to TH. [DUT as Client]</t>
+          <t>[TC-IDM-2.2] Report Data Action from DUT to TH. [DUT as Server]</t>
         </is>
       </c>
       <c r="D521" s="3" t="inlineStr">
         <is>
-          <t>TC-IDM-5.1</t>
+          <t>TC-IDM-2.2</t>
         </is>
       </c>
       <c r="E521" s="2" t="inlineStr">
@@ -13482,12 +13482,12 @@
       </c>
       <c r="C522" s="3" t="inlineStr">
         <is>
-          <t>[TC-IDM-5.2] Status Response from DUT in response to a Timed Request Action from TH.</t>
+          <t>[TC-IDM-3.1] Write Request Action from DUT to TH. [DUT as Client]</t>
         </is>
       </c>
       <c r="D522" s="3" t="inlineStr">
         <is>
-          <t>TC-IDM-5.2</t>
+          <t>TC-IDM-3.1</t>
         </is>
       </c>
       <c r="E522" s="2" t="inlineStr">
@@ -13507,12 +13507,12 @@
       </c>
       <c r="C523" s="3" t="inlineStr">
         <is>
-          <t>[TC-IDM-6.1] Events Read Interaction from TH to DUT. [DUT as Server]</t>
+          <t>[TC-IDM-3.2] Write Response Action from DUT to TH. [DUT as Server]</t>
         </is>
       </c>
       <c r="D523" s="3" t="inlineStr">
         <is>
-          <t>TC-IDM-6.1</t>
+          <t>TC-IDM-3.2</t>
         </is>
       </c>
       <c r="E523" s="2" t="inlineStr">
@@ -13532,12 +13532,12 @@
       </c>
       <c r="C524" s="3" t="inlineStr">
         <is>
-          <t>[TC-IDM-6.2] Events Subscribe Interaction from TH to DUT. [DUT as Server]</t>
+          <t>[TC-IDM-4.1] SubscriptionRequestMessage from DUT test cases. [DUT as Client]</t>
         </is>
       </c>
       <c r="D524" s="3" t="inlineStr">
         <is>
-          <t>TC-IDM-6.2</t>
+          <t>TC-IDM-4.1</t>
         </is>
       </c>
       <c r="E524" s="2" t="inlineStr">
@@ -13557,12 +13557,12 @@
       </c>
       <c r="C525" s="3" t="inlineStr">
         <is>
-          <t>[TC-IDM-6.3] Events Read Interaction from DUT to TH. [DUT as Client]</t>
+          <t>[TC-IDM-4.2] Subscription Response Messages from DUT Test Cases. [DUT as Server]</t>
         </is>
       </c>
       <c r="D525" s="3" t="inlineStr">
         <is>
-          <t>TC-IDM-6.3</t>
+          <t>TC-IDM-4.2</t>
         </is>
       </c>
       <c r="E525" s="2" t="inlineStr">
@@ -13582,12 +13582,12 @@
       </c>
       <c r="C526" s="3" t="inlineStr">
         <is>
-          <t>[TC-IDM-6.4] Events Subscribe Interaction from DUT to TH. [DUT as Client]</t>
+          <t>[TC-IDM-4.3] Report Data Messages post Subscription Activation from DUT Test Cases. [DUT as Server]</t>
         </is>
       </c>
       <c r="D526" s="3" t="inlineStr">
         <is>
-          <t>TC-IDM-6.4</t>
+          <t>TC-IDM-4.3</t>
         </is>
       </c>
       <c r="E526" s="2" t="inlineStr">
@@ -13607,12 +13607,12 @@
       </c>
       <c r="C527" s="3" t="inlineStr">
         <is>
-          <t>[TC-IDM-7.1] Multi Fabric Subscription Test Cases. [DUT as Server]</t>
+          <t>[TC-IDM-4.4] Persistent Subscription Test Cases. [DUT as Server]</t>
         </is>
       </c>
       <c r="D527" s="3" t="inlineStr">
         <is>
-          <t>TC-IDM-7.1</t>
+          <t>TC-IDM-4.4</t>
         </is>
       </c>
       <c r="E527" s="2" t="inlineStr">
@@ -13632,12 +13632,12 @@
       </c>
       <c r="C528" s="3" t="inlineStr">
         <is>
-          <t>[TC-IDM-8.1] Fabric scoped Test Cases. [DUT as Server]</t>
+          <t>[TC-IDM-5.1] Timed Request Action from DUT to TH. [DUT as Client]</t>
         </is>
       </c>
       <c r="D528" s="3" t="inlineStr">
         <is>
-          <t>TC-IDM-8.1</t>
+          <t>TC-IDM-5.1</t>
         </is>
       </c>
       <c r="E528" s="2" t="inlineStr">
@@ -13657,12 +13657,12 @@
       </c>
       <c r="C529" s="3" t="inlineStr">
         <is>
-          <t>[TC-IDM-9.1] CONSTRAINT_ERROR status response test cases [DUT as Server] - REMOVED</t>
+          <t>[TC-IDM-5.2] Status Response from DUT in response to a Timed Request Action from TH.</t>
         </is>
       </c>
       <c r="D529" s="3" t="inlineStr">
         <is>
-          <t>TC-IDM-9.1</t>
+          <t>TC-IDM-5.2</t>
         </is>
       </c>
       <c r="E529" s="2" t="inlineStr">
@@ -13682,12 +13682,12 @@
       </c>
       <c r="C530" s="3" t="inlineStr">
         <is>
-          <t>[TC-IDM-10.1] Cluster requirements - Global attributes [DUT as Server]</t>
+          <t>[TC-IDM-6.1] Events Read Interaction from TH to DUT. [DUT as Server]</t>
         </is>
       </c>
       <c r="D530" s="3" t="inlineStr">
         <is>
-          <t>TC-IDM-10.1</t>
+          <t>TC-IDM-6.1</t>
         </is>
       </c>
       <c r="E530" s="2" t="inlineStr">
@@ -13707,12 +13707,12 @@
       </c>
       <c r="C531" s="3" t="inlineStr">
         <is>
-          <t>[TC-IDM-11.1] Data types - attribute strings [DUT as Server] - data model</t>
+          <t>[TC-IDM-6.2] Events Subscribe Interaction from TH to DUT. [DUT as Server]</t>
         </is>
       </c>
       <c r="D531" s="3" t="inlineStr">
         <is>
-          <t>TC-IDM-11.1</t>
+          <t>TC-IDM-6.2</t>
         </is>
       </c>
       <c r="E531" s="2" t="inlineStr">
@@ -13727,17 +13727,17 @@
       </c>
       <c r="B532" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Administrator Commissioning </t>
+          <t>Interaction Data Model Test Plan</t>
         </is>
       </c>
       <c r="C532" s="3" t="inlineStr">
         <is>
-          <t>[TC-CADMIN-1.1] Administrator Behavior using ECM [DUT - Commissioner]</t>
+          <t>[TC-IDM-6.3] Events Read Interaction from DUT to TH. [DUT as Client]</t>
         </is>
       </c>
       <c r="D532" s="3" t="inlineStr">
         <is>
-          <t>TC-CADMIN-1.1</t>
+          <t>TC-IDM-6.3</t>
         </is>
       </c>
       <c r="E532" s="2" t="inlineStr">
@@ -13752,17 +13752,17 @@
       </c>
       <c r="B533" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Administrator Commissioning </t>
+          <t>Interaction Data Model Test Plan</t>
         </is>
       </c>
       <c r="C533" s="3" t="inlineStr">
         <is>
-          <t>[TC-CADMIN-1.2] Administrator Behavior using BCM [DUT - Commissioner]</t>
+          <t>[TC-IDM-6.4] Events Subscribe Interaction from DUT to TH. [DUT as Client]</t>
         </is>
       </c>
       <c r="D533" s="3" t="inlineStr">
         <is>
-          <t>TC-CADMIN-1.2</t>
+          <t>TC-IDM-6.4</t>
         </is>
       </c>
       <c r="E533" s="2" t="inlineStr">
@@ -13777,17 +13777,17 @@
       </c>
       <c r="B534" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Administrator Commissioning </t>
+          <t>Interaction Data Model Test Plan</t>
         </is>
       </c>
       <c r="C534" s="3" t="inlineStr">
         <is>
-          <t>[TC-CADMIN-1.3] Node Behavior using ECM [DUT - Commissionee]</t>
+          <t>[TC-IDM-7.1] Multi Fabric Subscription Test Cases. [DUT as Server]</t>
         </is>
       </c>
       <c r="D534" s="3" t="inlineStr">
         <is>
-          <t>TC-CADMIN-1.3</t>
+          <t>TC-IDM-7.1</t>
         </is>
       </c>
       <c r="E534" s="2" t="inlineStr">
@@ -13802,17 +13802,17 @@
       </c>
       <c r="B535" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Administrator Commissioning </t>
+          <t>Interaction Data Model Test Plan</t>
         </is>
       </c>
       <c r="C535" s="3" t="inlineStr">
         <is>
-          <t>[TC-CADMIN-1.4] Node Behavior using BCM [DUT - Commissionee]</t>
+          <t>[TC-IDM-8.1] Fabric scoped Test Cases. [DUT as Server]</t>
         </is>
       </c>
       <c r="D535" s="3" t="inlineStr">
         <is>
-          <t>TC-CADMIN-1.4</t>
+          <t>TC-IDM-8.1</t>
         </is>
       </c>
       <c r="E535" s="2" t="inlineStr">
@@ -13827,17 +13827,17 @@
       </c>
       <c r="B536" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Administrator Commissioning </t>
+          <t>Interaction Data Model Test Plan</t>
         </is>
       </c>
       <c r="C536" s="3" t="inlineStr">
         <is>
-          <t>[TC-CADMIN-1.5] Commissioning window handling timeout and revocation using ECM [DUT - Commissionee]</t>
+          <t>[TC-IDM-9.1] CONSTRAINT_ERROR status response test cases [DUT as Server] - REMOVED</t>
         </is>
       </c>
       <c r="D536" s="3" t="inlineStr">
         <is>
-          <t>TC-CADMIN-1.5</t>
+          <t>TC-IDM-9.1</t>
         </is>
       </c>
       <c r="E536" s="2" t="inlineStr">
@@ -13852,17 +13852,17 @@
       </c>
       <c r="B537" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Administrator Commissioning </t>
+          <t>Interaction Data Model Test Plan</t>
         </is>
       </c>
       <c r="C537" s="3" t="inlineStr">
         <is>
-          <t>[TC-CADMIN-1.6] Commissioning window handling timeout and revocation using BCM [DUT - Commissionee]</t>
+          <t>[TC-IDM-10.1] Cluster requirements - Global attributes [DUT as Server]</t>
         </is>
       </c>
       <c r="D537" s="3" t="inlineStr">
         <is>
-          <t>TC-CADMIN-1.6</t>
+          <t>TC-IDM-10.1</t>
         </is>
       </c>
       <c r="E537" s="2" t="inlineStr">
@@ -13877,17 +13877,17 @@
       </c>
       <c r="B538" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Administrator Commissioning </t>
+          <t>Interaction Data Model Test Plan</t>
         </is>
       </c>
       <c r="C538" s="3" t="inlineStr">
         <is>
-          <t>[TC-CADMIN-1.7] Commissioning window handling timeout and revocation using ECM [DUT - Commissioner]</t>
+          <t>[TC-IDM-11.1] Data types - attribute strings [DUT as Server] - data model</t>
         </is>
       </c>
       <c r="D538" s="3" t="inlineStr">
         <is>
-          <t>TC-CADMIN-1.7</t>
+          <t>TC-IDM-11.1</t>
         </is>
       </c>
       <c r="E538" s="2" t="inlineStr">
@@ -13907,12 +13907,12 @@
       </c>
       <c r="C539" s="3" t="inlineStr">
         <is>
-          <t>[TC-CADMIN-1.8] Commissioning window handling timeout and revocation using BCM [DUT - Commissioner]</t>
+          <t>[TC-CADMIN-1.1] Administrator Behavior using ECM [DUT - Commissioner]</t>
         </is>
       </c>
       <c r="D539" s="3" t="inlineStr">
         <is>
-          <t>TC-CADMIN-1.8</t>
+          <t>TC-CADMIN-1.1</t>
         </is>
       </c>
       <c r="E539" s="2" t="inlineStr">
@@ -13932,12 +13932,12 @@
       </c>
       <c r="C540" s="3" t="inlineStr">
         <is>
-          <t>[TC-CADMIN-1.9] Device exit commissioning mode after 20 failed commission attempts [ECM] [DUT - Commissionee]</t>
+          <t>[TC-CADMIN-1.2] Administrator Behavior using BCM [DUT - Commissioner]</t>
         </is>
       </c>
       <c r="D540" s="3" t="inlineStr">
         <is>
-          <t>TC-CADMIN-1.9</t>
+          <t>TC-CADMIN-1.2</t>
         </is>
       </c>
       <c r="E540" s="2" t="inlineStr">
@@ -13957,12 +13957,12 @@
       </c>
       <c r="C541" s="3" t="inlineStr">
         <is>
-          <t>[TC-CADMIN-1.10] Device exit commissioning mode after 20 failed commission attempts [BCM] [DUT - Commissionee]</t>
+          <t>[TC-CADMIN-1.3] Node Behavior using ECM [DUT - Commissionee]</t>
         </is>
       </c>
       <c r="D541" s="3" t="inlineStr">
         <is>
-          <t>TC-CADMIN-1.10</t>
+          <t>TC-CADMIN-1.3</t>
         </is>
       </c>
       <c r="E541" s="2" t="inlineStr">
@@ -13982,12 +13982,12 @@
       </c>
       <c r="C542" s="3" t="inlineStr">
         <is>
-          <t>[TC-CADMIN-1.11] Open commissioning window on DUT twice using ECM then BCM [DUT - Commissionee]</t>
+          <t>[TC-CADMIN-1.4] Node Behavior using BCM [DUT - Commissionee]</t>
         </is>
       </c>
       <c r="D542" s="3" t="inlineStr">
         <is>
-          <t>TC-CADMIN-1.11</t>
+          <t>TC-CADMIN-1.4</t>
         </is>
       </c>
       <c r="E542" s="2" t="inlineStr">
@@ -14007,12 +14007,12 @@
       </c>
       <c r="C543" s="3" t="inlineStr">
         <is>
-          <t>[TC-CADMIN-1.12] Open commissioning window on DUT twice using ECM then BCM [DUT - Commissioner]</t>
+          <t>[TC-CADMIN-1.5] Commissioning window handling timeout and revocation using ECM [DUT - Commissionee]</t>
         </is>
       </c>
       <c r="D543" s="3" t="inlineStr">
         <is>
-          <t>TC-CADMIN-1.12</t>
+          <t>TC-CADMIN-1.5</t>
         </is>
       </c>
       <c r="E543" s="2" t="inlineStr">
@@ -14032,12 +14032,12 @@
       </c>
       <c r="C544" s="3" t="inlineStr">
         <is>
-          <t>[TC-CADMIN-1.13] Open commissioning window twice on DUT using BCM then ECM [DUT - Commissionee]</t>
+          <t>[TC-CADMIN-1.6] Commissioning window handling timeout and revocation using BCM [DUT - Commissionee]</t>
         </is>
       </c>
       <c r="D544" s="3" t="inlineStr">
         <is>
-          <t>TC-CADMIN-1.13</t>
+          <t>TC-CADMIN-1.6</t>
         </is>
       </c>
       <c r="E544" s="2" t="inlineStr">
@@ -14057,12 +14057,12 @@
       </c>
       <c r="C545" s="3" t="inlineStr">
         <is>
-          <t>[TC-CADMIN-1.14] Open commissioning window twice on DUT using BCM then ECM [DUT - Commissioner]</t>
+          <t>[TC-CADMIN-1.7] Commissioning window handling timeout and revocation using ECM [DUT - Commissioner]</t>
         </is>
       </c>
       <c r="D545" s="3" t="inlineStr">
         <is>
-          <t>TC-CADMIN-1.14</t>
+          <t>TC-CADMIN-1.7</t>
         </is>
       </c>
       <c r="E545" s="2" t="inlineStr">
@@ -14082,12 +14082,12 @@
       </c>
       <c r="C546" s="3" t="inlineStr">
         <is>
-          <t>[TC-CADMIN-1.15] Removing Fabrics from DUT and Fabric index enumeration using ECM [DUT - Commissionee]</t>
+          <t>[TC-CADMIN-1.8] Commissioning window handling timeout and revocation using BCM [DUT - Commissioner]</t>
         </is>
       </c>
       <c r="D546" s="3" t="inlineStr">
         <is>
-          <t>TC-CADMIN-1.15</t>
+          <t>TC-CADMIN-1.8</t>
         </is>
       </c>
       <c r="E546" s="2" t="inlineStr">
@@ -14107,12 +14107,12 @@
       </c>
       <c r="C547" s="3" t="inlineStr">
         <is>
-          <t>[TC-CADMIN-1.16] Removing Fabrics from DUT and Fabric index enumeration using BCM [DUT - Commissionee]</t>
+          <t>[TC-CADMIN-1.9] Device exit commissioning mode after 20 failed commission attempts [ECM] [DUT - Commissionee]</t>
         </is>
       </c>
       <c r="D547" s="3" t="inlineStr">
         <is>
-          <t>TC-CADMIN-1.16</t>
+          <t>TC-CADMIN-1.9</t>
         </is>
       </c>
       <c r="E547" s="2" t="inlineStr">
@@ -14132,12 +14132,12 @@
       </c>
       <c r="C548" s="3" t="inlineStr">
         <is>
-          <t>[TC-CADMIN-1.17] Removing Fabrics from DUT and Fabric index enumeration using ECM [DUT - Commissioner]</t>
+          <t>[TC-CADMIN-1.10] Device exit commissioning mode after 20 failed commission attempts [BCM] [DUT - Commissionee]</t>
         </is>
       </c>
       <c r="D548" s="3" t="inlineStr">
         <is>
-          <t>TC-CADMIN-1.17</t>
+          <t>TC-CADMIN-1.10</t>
         </is>
       </c>
       <c r="E548" s="2" t="inlineStr">
@@ -14157,12 +14157,12 @@
       </c>
       <c r="C549" s="3" t="inlineStr">
         <is>
-          <t>[TC-CADMIN-1.18] Removing Fabrics from DUT and Fabric index enumeration using BCM [DUT - Commissioner]</t>
+          <t>[TC-CADMIN-1.11] Open commissioning window on DUT twice using ECM then BCM [DUT - Commissionee]</t>
         </is>
       </c>
       <c r="D549" s="3" t="inlineStr">
         <is>
-          <t>TC-CADMIN-1.18</t>
+          <t>TC-CADMIN-1.11</t>
         </is>
       </c>
       <c r="E549" s="2" t="inlineStr">
@@ -14182,12 +14182,12 @@
       </c>
       <c r="C550" s="3" t="inlineStr">
         <is>
-          <t>[TC-CADMIN-1.19] max number of Commissioned Fabrics and SupportedFabrics rollover using ECM [DUT - Commissionee]</t>
+          <t>[TC-CADMIN-1.12] Open commissioning window on DUT twice using ECM then BCM [DUT - Commissioner]</t>
         </is>
       </c>
       <c r="D550" s="3" t="inlineStr">
         <is>
-          <t>TC-CADMIN-1.19</t>
+          <t>TC-CADMIN-1.12</t>
         </is>
       </c>
       <c r="E550" s="2" t="inlineStr">
@@ -14207,12 +14207,12 @@
       </c>
       <c r="C551" s="3" t="inlineStr">
         <is>
-          <t>[TC-CADMIN-1.20] max number of Commissioned Fabrics and SupportedFabrics rollover using BCM [DUT - Commissionee]</t>
+          <t>[TC-CADMIN-1.13] Open commissioning window twice on DUT using BCM then ECM [DUT - Commissionee]</t>
         </is>
       </c>
       <c r="D551" s="3" t="inlineStr">
         <is>
-          <t>TC-CADMIN-1.20</t>
+          <t>TC-CADMIN-1.13</t>
         </is>
       </c>
       <c r="E551" s="2" t="inlineStr">
@@ -14232,12 +14232,12 @@
       </c>
       <c r="C552" s="3" t="inlineStr">
         <is>
-          <t>[TC-CADMIN-1.21] Open commissioning window - durations max and max+1 [BCM] [DUT - Commissionee]</t>
+          <t>[TC-CADMIN-1.14] Open commissioning window twice on DUT using BCM then ECM [DUT - Commissioner]</t>
         </is>
       </c>
       <c r="D552" s="3" t="inlineStr">
         <is>
-          <t>TC-CADMIN-1.21</t>
+          <t>TC-CADMIN-1.14</t>
         </is>
       </c>
       <c r="E552" s="2" t="inlineStr">
@@ -14257,12 +14257,12 @@
       </c>
       <c r="C553" s="3" t="inlineStr">
         <is>
-          <t>[TC-CADMIN-1.22] Open commissioning window - durations max and max+1 [ECM] [DUT - Commissionee]</t>
+          <t>[TC-CADMIN-1.15] Removing Fabrics from DUT and Fabric index enumeration using ECM [DUT - Commissionee]</t>
         </is>
       </c>
       <c r="D553" s="3" t="inlineStr">
         <is>
-          <t>TC-CADMIN-1.22</t>
+          <t>TC-CADMIN-1.15</t>
         </is>
       </c>
       <c r="E553" s="2" t="inlineStr">
@@ -14282,12 +14282,12 @@
       </c>
       <c r="C554" s="3" t="inlineStr">
         <is>
-          <t>[TC-CADMIN-1.23] Open commissioning window - durations min and min-1 [BCM] [DUT - Commissionee]</t>
+          <t>[TC-CADMIN-1.16] Removing Fabrics from DUT and Fabric index enumeration using BCM [DUT - Commissionee]</t>
         </is>
       </c>
       <c r="D554" s="3" t="inlineStr">
         <is>
-          <t>TC-CADMIN-1.23</t>
+          <t>TC-CADMIN-1.16</t>
         </is>
       </c>
       <c r="E554" s="2" t="inlineStr">
@@ -14307,12 +14307,12 @@
       </c>
       <c r="C555" s="3" t="inlineStr">
         <is>
-          <t>[TC-CADMIN-1.24] Open commissioning window - durations min and min-1 [ECM] [DUT - Commissionee]</t>
+          <t>[TC-CADMIN-1.17] Removing Fabrics from DUT and Fabric index enumeration using ECM [DUT - Commissioner]</t>
         </is>
       </c>
       <c r="D555" s="3" t="inlineStr">
         <is>
-          <t>TC-CADMIN-1.24</t>
+          <t>TC-CADMIN-1.17</t>
         </is>
       </c>
       <c r="E555" s="2" t="inlineStr">
@@ -14332,12 +14332,12 @@
       </c>
       <c r="C556" s="3" t="inlineStr">
         <is>
-          <t>[TC-CADMIN-1.25] Subscription to the attributes - verify subscription response [ECM] [DUT - Commissionee]</t>
+          <t>[TC-CADMIN-1.18] Removing Fabrics from DUT and Fabric index enumeration using BCM [DUT - Commissioner]</t>
         </is>
       </c>
       <c r="D556" s="3" t="inlineStr">
         <is>
-          <t>TC-CADMIN-1.25</t>
+          <t>TC-CADMIN-1.18</t>
         </is>
       </c>
       <c r="E556" s="2" t="inlineStr">
@@ -14357,12 +14357,12 @@
       </c>
       <c r="C557" s="3" t="inlineStr">
         <is>
-          <t>[TC-CADMIN-1.26] Subscription to the attributes - verify subscription response [BCM] [DUT - Commissionee]</t>
+          <t>[TC-CADMIN-1.19] max number of Commissioned Fabrics and SupportedFabrics rollover using ECM [DUT - Commissionee]</t>
         </is>
       </c>
       <c r="D557" s="3" t="inlineStr">
         <is>
-          <t>TC-CADMIN-1.26</t>
+          <t>TC-CADMIN-1.19</t>
         </is>
       </c>
       <c r="E557" s="2" t="inlineStr">
@@ -14377,17 +14377,17 @@
       </c>
       <c r="B558" s="3" t="inlineStr">
         <is>
-          <t>Bridge Test Plan</t>
+          <t xml:space="preserve">Administrator Commissioning </t>
         </is>
       </c>
       <c r="C558" s="3" t="inlineStr">
         <is>
-          <t>[TC-BR-1] Basics of bridging (DUT server)</t>
+          <t>[TC-CADMIN-1.20] max number of Commissioned Fabrics and SupportedFabrics rollover using BCM [DUT - Commissionee]</t>
         </is>
       </c>
       <c r="D558" s="3" t="inlineStr">
         <is>
-          <t>TC-BR-1</t>
+          <t>TC-CADMIN-1.20</t>
         </is>
       </c>
       <c r="E558" s="2" t="inlineStr">
@@ -14402,17 +14402,17 @@
       </c>
       <c r="B559" s="3" t="inlineStr">
         <is>
-          <t>Bridge Test Plan</t>
+          <t xml:space="preserve">Administrator Commissioning </t>
         </is>
       </c>
       <c r="C559" s="3" t="inlineStr">
         <is>
-          <t>[TC-BR-2] Changing the set of bridged devices (DUT server)</t>
+          <t>[TC-CADMIN-1.21] Open commissioning window - durations max and max+1 [BCM] [DUT - Commissionee]</t>
         </is>
       </c>
       <c r="D559" s="3" t="inlineStr">
         <is>
-          <t>TC-BR-2</t>
+          <t>TC-CADMIN-1.21</t>
         </is>
       </c>
       <c r="E559" s="2" t="inlineStr">
@@ -14427,17 +14427,17 @@
       </c>
       <c r="B560" s="3" t="inlineStr">
         <is>
-          <t>Bridge Test Plan</t>
+          <t xml:space="preserve">Administrator Commissioning </t>
         </is>
       </c>
       <c r="C560" s="3" t="inlineStr">
         <is>
-          <t>[TC-BR-3] Changing name and state of a bridged device (DUT server)</t>
+          <t>[TC-CADMIN-1.22] Open commissioning window - durations max and max+1 [ECM] [DUT - Commissionee]</t>
         </is>
       </c>
       <c r="D560" s="3" t="inlineStr">
         <is>
-          <t>TC-BR-3</t>
+          <t>TC-CADMIN-1.22</t>
         </is>
       </c>
       <c r="E560" s="2" t="inlineStr">
@@ -14452,17 +14452,17 @@
       </c>
       <c r="B561" s="3" t="inlineStr">
         <is>
-          <t>Bridge Test Plan</t>
+          <t xml:space="preserve">Administrator Commissioning </t>
         </is>
       </c>
       <c r="C561" s="3" t="inlineStr">
         <is>
-          <t>[TC-BR-4] DUT client handling of bridges (DUT client)</t>
+          <t>[TC-CADMIN-1.23] Open commissioning window - durations min and min-1 [BCM] [DUT - Commissionee]</t>
         </is>
       </c>
       <c r="D561" s="3" t="inlineStr">
         <is>
-          <t>TC-BR-4</t>
+          <t>TC-CADMIN-1.23</t>
         </is>
       </c>
       <c r="E561" s="2" t="inlineStr">
@@ -14477,17 +14477,17 @@
       </c>
       <c r="B562" s="3" t="inlineStr">
         <is>
-          <t>Bulk Data Exchange Protocol Test Plan</t>
+          <t xml:space="preserve">Administrator Commissioning </t>
         </is>
       </c>
       <c r="C562" s="3" t="inlineStr">
         <is>
-          <t>[TC-BDX-1.1] Sender Initiated BDX Transfer Session - REMOVED</t>
+          <t>[TC-CADMIN-1.24] Open commissioning window - durations min and min-1 [ECM] [DUT - Commissionee]</t>
         </is>
       </c>
       <c r="D562" s="3" t="inlineStr">
         <is>
-          <t>TC-BDX-1.1</t>
+          <t>TC-CADMIN-1.24</t>
         </is>
       </c>
       <c r="E562" s="2" t="inlineStr">
@@ -14502,17 +14502,17 @@
       </c>
       <c r="B563" s="3" t="inlineStr">
         <is>
-          <t>Bulk Data Exchange Protocol Test Plan</t>
+          <t xml:space="preserve">Administrator Commissioning </t>
         </is>
       </c>
       <c r="C563" s="3" t="inlineStr">
         <is>
-          <t>[TC-BDX-1.2] Receiver Initiated BDX Transfer Session</t>
+          <t>[TC-CADMIN-1.25] Subscription to the attributes - verify subscription response [ECM] [DUT - Commissionee]</t>
         </is>
       </c>
       <c r="D563" s="3" t="inlineStr">
         <is>
-          <t>TC-BDX-1.2</t>
+          <t>TC-CADMIN-1.25</t>
         </is>
       </c>
       <c r="E563" s="2" t="inlineStr">
@@ -14527,17 +14527,17 @@
       </c>
       <c r="B564" s="3" t="inlineStr">
         <is>
-          <t>Bulk Data Exchange Protocol Test Plan</t>
+          <t xml:space="preserve">Administrator Commissioning </t>
         </is>
       </c>
       <c r="C564" s="3" t="inlineStr">
         <is>
-          <t>[TC-BDX-1.3] Response to Sender Initiated BDX Transfer Session - REMOVED</t>
+          <t>[TC-CADMIN-1.26] Subscription to the attributes - verify subscription response [BCM] [DUT - Commissionee]</t>
         </is>
       </c>
       <c r="D564" s="3" t="inlineStr">
         <is>
-          <t>TC-BDX-1.3</t>
+          <t>TC-CADMIN-1.26</t>
         </is>
       </c>
       <c r="E564" s="2" t="inlineStr">
@@ -14552,17 +14552,17 @@
       </c>
       <c r="B565" s="3" t="inlineStr">
         <is>
-          <t>Bulk Data Exchange Protocol Test Plan</t>
+          <t>Bridge Test Plan</t>
         </is>
       </c>
       <c r="C565" s="3" t="inlineStr">
         <is>
-          <t>[TC-BDX-1.4] Response to Receiver Initiated BDX Transfer Session</t>
+          <t>[TC-BR-1] Basics of bridging (DUT server)</t>
         </is>
       </c>
       <c r="D565" s="3" t="inlineStr">
         <is>
-          <t>TC-BDX-1.4</t>
+          <t>TC-BR-1</t>
         </is>
       </c>
       <c r="E565" s="2" t="inlineStr">
@@ -14577,17 +14577,17 @@
       </c>
       <c r="B566" s="3" t="inlineStr">
         <is>
-          <t>Bulk Data Exchange Protocol Test Plan</t>
+          <t>Bridge Test Plan</t>
         </is>
       </c>
       <c r="C566" s="3" t="inlineStr">
         <is>
-          <t>[TC-BDX-1.5] Response to Sender Initiated BDX Transfer Session - Negative Scenario - REMOVED</t>
+          <t>[TC-BR-2] Changing the set of bridged devices (DUT server)</t>
         </is>
       </c>
       <c r="D566" s="3" t="inlineStr">
         <is>
-          <t>TC-BDX-1.5</t>
+          <t>TC-BR-2</t>
         </is>
       </c>
       <c r="E566" s="2" t="inlineStr">
@@ -14602,17 +14602,17 @@
       </c>
       <c r="B567" s="3" t="inlineStr">
         <is>
-          <t>Bulk Data Exchange Protocol Test Plan</t>
+          <t>Bridge Test Plan</t>
         </is>
       </c>
       <c r="C567" s="3" t="inlineStr">
         <is>
-          <t>[TC-BDX-1.6] Response to Receiver Initiated BDX Transfer Session - Negative Scenario - REMOVED</t>
+          <t>[TC-BR-3] Changing name and state of a bridged device (DUT server)</t>
         </is>
       </c>
       <c r="D567" s="3" t="inlineStr">
         <is>
-          <t>TC-BDX-1.6</t>
+          <t>TC-BR-3</t>
         </is>
       </c>
       <c r="E567" s="2" t="inlineStr">
@@ -14627,17 +14627,17 @@
       </c>
       <c r="B568" s="3" t="inlineStr">
         <is>
-          <t>Bulk Data Exchange Protocol Test Plan</t>
+          <t>Bridge Test Plan</t>
         </is>
       </c>
       <c r="C568" s="3" t="inlineStr">
         <is>
-          <t>[TC-BDX-2.1] Synchronous File Sending</t>
+          <t>[TC-BR-4] DUT client handling of bridges (DUT client)</t>
         </is>
       </c>
       <c r="D568" s="3" t="inlineStr">
         <is>
-          <t>TC-BDX-2.1</t>
+          <t>TC-BR-4</t>
         </is>
       </c>
       <c r="E568" s="2" t="inlineStr">
@@ -14657,12 +14657,12 @@
       </c>
       <c r="C569" s="3" t="inlineStr">
         <is>
-          <t>[TC-BDX-2.2] Synchronous File Receiving</t>
+          <t>[TC-BDX-1.1] Sender Initiated BDX Transfer Session - REMOVED</t>
         </is>
       </c>
       <c r="D569" s="3" t="inlineStr">
         <is>
-          <t>TC-BDX-2.2</t>
+          <t>TC-BDX-1.1</t>
         </is>
       </c>
       <c r="E569" s="2" t="inlineStr">
@@ -14682,12 +14682,12 @@
       </c>
       <c r="C570" s="3" t="inlineStr">
         <is>
-          <t>[TC-BDX-2.3] Restart Synchronous File Receiving - REMOVED</t>
+          <t>[TC-BDX-1.2] Receiver Initiated BDX Transfer Session</t>
         </is>
       </c>
       <c r="D570" s="3" t="inlineStr">
         <is>
-          <t>TC-BDX-2.3</t>
+          <t>TC-BDX-1.2</t>
         </is>
       </c>
       <c r="E570" s="2" t="inlineStr">
@@ -14707,12 +14707,12 @@
       </c>
       <c r="C571" s="3" t="inlineStr">
         <is>
-          <t>[TC-BDX-2.4] Asynchronous File Sending - REMOVED</t>
+          <t>[TC-BDX-1.3] Response to Sender Initiated BDX Transfer Session - REMOVED</t>
         </is>
       </c>
       <c r="D571" s="3" t="inlineStr">
         <is>
-          <t>TC-BDX-2.4</t>
+          <t>TC-BDX-1.3</t>
         </is>
       </c>
       <c r="E571" s="2" t="inlineStr">
@@ -14732,12 +14732,12 @@
       </c>
       <c r="C572" s="3" t="inlineStr">
         <is>
-          <t>[TC-BDX-2.5] Asynchronous File Receiving - REMOVED</t>
+          <t>[TC-BDX-1.4] Response to Receiver Initiated BDX Transfer Session</t>
         </is>
       </c>
       <c r="D572" s="3" t="inlineStr">
         <is>
-          <t>TC-BDX-2.5</t>
+          <t>TC-BDX-1.4</t>
         </is>
       </c>
       <c r="E572" s="2" t="inlineStr">
@@ -14752,17 +14752,17 @@
       </c>
       <c r="B573" s="3" t="inlineStr">
         <is>
-          <t>OTA Software Update Test Plan</t>
+          <t>Bulk Data Exchange Protocol Test Plan</t>
         </is>
       </c>
       <c r="C573" s="3" t="inlineStr">
         <is>
-          <t>[TC-SU-1.1] Invoke AnnounceOTAProvider from Admin(DUT) to OTA-R</t>
+          <t>[TC-BDX-1.5] Response to Sender Initiated BDX Transfer Session - Negative Scenario - REMOVED</t>
         </is>
       </c>
       <c r="D573" s="3" t="inlineStr">
         <is>
-          <t>TC-SU-1.1</t>
+          <t>TC-BDX-1.5</t>
         </is>
       </c>
       <c r="E573" s="2" t="inlineStr">
@@ -14777,17 +14777,17 @@
       </c>
       <c r="B574" s="3" t="inlineStr">
         <is>
-          <t>OTA Software Update Test Plan</t>
+          <t>Bulk Data Exchange Protocol Test Plan</t>
         </is>
       </c>
       <c r="C574" s="3" t="inlineStr">
         <is>
-          <t>[TC-SU-2.1] QueryImage Command from DUT to OTA-P</t>
+          <t>[TC-BDX-1.6] Response to Receiver Initiated BDX Transfer Session - Negative Scenario - REMOVED</t>
         </is>
       </c>
       <c r="D574" s="3" t="inlineStr">
         <is>
-          <t>TC-SU-2.1</t>
+          <t>TC-BDX-1.6</t>
         </is>
       </c>
       <c r="E574" s="2" t="inlineStr">
@@ -14802,17 +14802,17 @@
       </c>
       <c r="B575" s="3" t="inlineStr">
         <is>
-          <t>OTA Software Update Test Plan</t>
+          <t>Bulk Data Exchange Protocol Test Plan</t>
         </is>
       </c>
       <c r="C575" s="3" t="inlineStr">
         <is>
-          <t>[TC-SU-2.2] Handling Different QueryImageResponse Scenarios on Requestor</t>
+          <t>[TC-BDX-2.1] Synchronous File Sending</t>
         </is>
       </c>
       <c r="D575" s="3" t="inlineStr">
         <is>
-          <t>TC-SU-2.2</t>
+          <t>TC-BDX-2.1</t>
         </is>
       </c>
       <c r="E575" s="2" t="inlineStr">
@@ -14827,17 +14827,17 @@
       </c>
       <c r="B576" s="3" t="inlineStr">
         <is>
-          <t>OTA Software Update Test Plan</t>
+          <t>Bulk Data Exchange Protocol Test Plan</t>
         </is>
       </c>
       <c r="C576" s="3" t="inlineStr">
         <is>
-          <t>[TC-SU-2.3] Transfer of Software Update Images between DUT and TH/OTA-P</t>
+          <t>[TC-BDX-2.2] Synchronous File Receiving</t>
         </is>
       </c>
       <c r="D576" s="3" t="inlineStr">
         <is>
-          <t>TC-SU-2.3</t>
+          <t>TC-BDX-2.2</t>
         </is>
       </c>
       <c r="E576" s="2" t="inlineStr">
@@ -14852,17 +14852,17 @@
       </c>
       <c r="B577" s="3" t="inlineStr">
         <is>
-          <t>OTA Software Update Test Plan</t>
+          <t>Bulk Data Exchange Protocol Test Plan</t>
         </is>
       </c>
       <c r="C577" s="3" t="inlineStr">
         <is>
-          <t>[TC-SU-2.4] ApplyUpdateRequest Command from DUT to OTA-P</t>
+          <t>[TC-BDX-2.3] Restart Synchronous File Receiving - REMOVED</t>
         </is>
       </c>
       <c r="D577" s="3" t="inlineStr">
         <is>
-          <t>TC-SU-2.4</t>
+          <t>TC-BDX-2.3</t>
         </is>
       </c>
       <c r="E577" s="2" t="inlineStr">
@@ -14877,17 +14877,17 @@
       </c>
       <c r="B578" s="3" t="inlineStr">
         <is>
-          <t>OTA Software Update Test Plan</t>
+          <t>Bulk Data Exchange Protocol Test Plan</t>
         </is>
       </c>
       <c r="C578" s="3" t="inlineStr">
         <is>
-          <t>[TC-SU-2.5] Handling Different ApplyUpdateResponse Scenarios on Requestor</t>
+          <t>[TC-BDX-2.4] Asynchronous File Sending - REMOVED</t>
         </is>
       </c>
       <c r="D578" s="3" t="inlineStr">
         <is>
-          <t>TC-SU-2.5</t>
+          <t>TC-BDX-2.4</t>
         </is>
       </c>
       <c r="E578" s="2" t="inlineStr">
@@ -14902,17 +14902,17 @@
       </c>
       <c r="B579" s="3" t="inlineStr">
         <is>
-          <t>OTA Software Update Test Plan</t>
+          <t>Bulk Data Exchange Protocol Test Plan</t>
         </is>
       </c>
       <c r="C579" s="3" t="inlineStr">
         <is>
-          <t>[TC-SU-2.6] NotifyUpdateApplied Command from DUT to OTA-P</t>
+          <t>[TC-BDX-2.5] Asynchronous File Receiving - REMOVED</t>
         </is>
       </c>
       <c r="D579" s="3" t="inlineStr">
         <is>
-          <t>TC-SU-2.6</t>
+          <t>TC-BDX-2.5</t>
         </is>
       </c>
       <c r="E579" s="2" t="inlineStr">
@@ -14932,12 +14932,12 @@
       </c>
       <c r="C580" s="3" t="inlineStr">
         <is>
-          <t>[TC-SU-2.7] Verifying Events on OTA-R(DUT)</t>
+          <t>[TC-SU-1.1] Invoke AnnounceOTAProvider from Admin(DUT) to OTA-R</t>
         </is>
       </c>
       <c r="D580" s="3" t="inlineStr">
         <is>
-          <t>TC-SU-2.7</t>
+          <t>TC-SU-1.1</t>
         </is>
       </c>
       <c r="E580" s="2" t="inlineStr">
@@ -14957,12 +14957,12 @@
       </c>
       <c r="C581" s="3" t="inlineStr">
         <is>
-          <t>[TC-SU-2.8] OTA Functionality in Multi Fabric Scenario</t>
+          <t>[TC-SU-2.1] QueryImage Command from DUT to OTA-P</t>
         </is>
       </c>
       <c r="D581" s="3" t="inlineStr">
         <is>
-          <t>TC-SU-2.8</t>
+          <t>TC-SU-2.1</t>
         </is>
       </c>
       <c r="E581" s="2" t="inlineStr">
@@ -14982,12 +14982,12 @@
       </c>
       <c r="C582" s="3" t="inlineStr">
         <is>
-          <t>[TC-SU-3.1] QueryImageResponse from DUT to OTA-R</t>
+          <t>[TC-SU-2.2] Handling Different QueryImageResponse Scenarios on Requestor</t>
         </is>
       </c>
       <c r="D582" s="3" t="inlineStr">
         <is>
-          <t>TC-SU-3.1</t>
+          <t>TC-SU-2.2</t>
         </is>
       </c>
       <c r="E582" s="2" t="inlineStr">
@@ -15007,12 +15007,12 @@
       </c>
       <c r="C583" s="3" t="inlineStr">
         <is>
-          <t>[TC-SU-3.2] Handling Different QueryImageResponse Scenarios on Provider</t>
+          <t>[TC-SU-2.3] Transfer of Software Update Images between DUT and TH/OTA-P</t>
         </is>
       </c>
       <c r="D583" s="3" t="inlineStr">
         <is>
-          <t>TC-SU-3.2</t>
+          <t>TC-SU-2.3</t>
         </is>
       </c>
       <c r="E583" s="2" t="inlineStr">
@@ -15032,12 +15032,12 @@
       </c>
       <c r="C584" s="3" t="inlineStr">
         <is>
-          <t>[TC-SU-3.3] Transfer of Software Update Images between DUT and OTA-R</t>
+          <t>[TC-SU-2.4] ApplyUpdateRequest Command from DUT to OTA-P</t>
         </is>
       </c>
       <c r="D584" s="3" t="inlineStr">
         <is>
-          <t>TC-SU-3.3</t>
+          <t>TC-SU-2.4</t>
         </is>
       </c>
       <c r="E584" s="2" t="inlineStr">
@@ -15057,12 +15057,12 @@
       </c>
       <c r="C585" s="3" t="inlineStr">
         <is>
-          <t>[TC-SU-3.4] Handling Different ApplyUpdateResponse Scenarios on Provider</t>
+          <t>[TC-SU-2.5] Handling Different ApplyUpdateResponse Scenarios on Requestor</t>
         </is>
       </c>
       <c r="D585" s="3" t="inlineStr">
         <is>
-          <t>TC-SU-3.4</t>
+          <t>TC-SU-2.5</t>
         </is>
       </c>
       <c r="E585" s="2" t="inlineStr">
@@ -15082,12 +15082,12 @@
       </c>
       <c r="C586" s="3" t="inlineStr">
         <is>
-          <t>[TC-SU-4.1] Verifying Cluster Attributes on OTA-R(DUT)</t>
+          <t>[TC-SU-2.6] NotifyUpdateApplied Command from DUT to OTA-P</t>
         </is>
       </c>
       <c r="D586" s="3" t="inlineStr">
         <is>
-          <t>TC-SU-4.1</t>
+          <t>TC-SU-2.6</t>
         </is>
       </c>
       <c r="E586" s="2" t="inlineStr">
@@ -15107,12 +15107,12 @@
       </c>
       <c r="C587" s="3" t="inlineStr">
         <is>
-          <t>[TC-SU-4.2] Verifying Cluster Attributes from Admin(DUT)</t>
+          <t>[TC-SU-2.7] Verifying Events on OTA-R(DUT)</t>
         </is>
       </c>
       <c r="D587" s="3" t="inlineStr">
         <is>
-          <t>TC-SU-4.2</t>
+          <t>TC-SU-2.7</t>
         </is>
       </c>
       <c r="E587" s="2" t="inlineStr">
@@ -15127,17 +15127,17 @@
       </c>
       <c r="B588" s="3" t="inlineStr">
         <is>
-          <t>Access Control Enforcement Test Plan</t>
+          <t>OTA Software Update Test Plan</t>
         </is>
       </c>
       <c r="C588" s="3" t="inlineStr">
         <is>
-          <t>[TC-ACE-1.1] Privileges</t>
+          <t>[TC-SU-2.8] OTA Functionality in Multi Fabric Scenario</t>
         </is>
       </c>
       <c r="D588" s="3" t="inlineStr">
         <is>
-          <t>TC-ACE-1.1</t>
+          <t>TC-SU-2.8</t>
         </is>
       </c>
       <c r="E588" s="2" t="inlineStr">
@@ -15152,17 +15152,17 @@
       </c>
       <c r="B589" s="3" t="inlineStr">
         <is>
-          <t>Access Control Enforcement Test Plan</t>
+          <t>OTA Software Update Test Plan</t>
         </is>
       </c>
       <c r="C589" s="3" t="inlineStr">
         <is>
-          <t>[TC-ACE-1.2] Subscriptions</t>
+          <t>[TC-SU-3.1] QueryImageResponse from DUT to OTA-R</t>
         </is>
       </c>
       <c r="D589" s="3" t="inlineStr">
         <is>
-          <t>TC-ACE-1.2</t>
+          <t>TC-SU-3.1</t>
         </is>
       </c>
       <c r="E589" s="2" t="inlineStr">
@@ -15177,17 +15177,17 @@
       </c>
       <c r="B590" s="3" t="inlineStr">
         <is>
-          <t>Access Control Enforcement Test Plan</t>
+          <t>OTA Software Update Test Plan</t>
         </is>
       </c>
       <c r="C590" s="3" t="inlineStr">
         <is>
-          <t>[TC-ACE-1.3] Subjects</t>
+          <t>[TC-SU-3.2] Handling Different QueryImageResponse Scenarios on Provider</t>
         </is>
       </c>
       <c r="D590" s="3" t="inlineStr">
         <is>
-          <t>TC-ACE-1.3</t>
+          <t>TC-SU-3.2</t>
         </is>
       </c>
       <c r="E590" s="2" t="inlineStr">
@@ -15202,17 +15202,17 @@
       </c>
       <c r="B591" s="3" t="inlineStr">
         <is>
-          <t>Access Control Enforcement Test Plan</t>
+          <t>OTA Software Update Test Plan</t>
         </is>
       </c>
       <c r="C591" s="3" t="inlineStr">
         <is>
-          <t>[TC-ACE-1.4] Targets</t>
+          <t>[TC-SU-3.3] Transfer of Software Update Images between DUT and OTA-R</t>
         </is>
       </c>
       <c r="D591" s="3" t="inlineStr">
         <is>
-          <t>TC-ACE-1.4</t>
+          <t>TC-SU-3.3</t>
         </is>
       </c>
       <c r="E591" s="2" t="inlineStr">
@@ -15227,17 +15227,17 @@
       </c>
       <c r="B592" s="3" t="inlineStr">
         <is>
-          <t>Access Control Enforcement Test Plan</t>
+          <t>OTA Software Update Test Plan</t>
         </is>
       </c>
       <c r="C592" s="3" t="inlineStr">
         <is>
-          <t>[TC-ACE-1.5] Multi-fabric</t>
+          <t>[TC-SU-3.4] Handling Different ApplyUpdateResponse Scenarios on Provider</t>
         </is>
       </c>
       <c r="D592" s="3" t="inlineStr">
         <is>
-          <t>TC-ACE-1.5</t>
+          <t>TC-SU-3.4</t>
         </is>
       </c>
       <c r="E592" s="2" t="inlineStr">
@@ -15252,17 +15252,17 @@
       </c>
       <c r="B593" s="3" t="inlineStr">
         <is>
-          <t>Access Control Enforcement Test Plan</t>
+          <t>OTA Software Update Test Plan</t>
         </is>
       </c>
       <c r="C593" s="3" t="inlineStr">
         <is>
-          <t>[TC-ACE-1.6] Group auth mode</t>
+          <t>[TC-SU-4.1] Verifying Cluster Attributes on OTA-R(DUT)</t>
         </is>
       </c>
       <c r="D593" s="3" t="inlineStr">
         <is>
-          <t>TC-ACE-1.6</t>
+          <t>TC-SU-4.1</t>
         </is>
       </c>
       <c r="E593" s="2" t="inlineStr">
@@ -15277,17 +15277,17 @@
       </c>
       <c r="B594" s="3" t="inlineStr">
         <is>
-          <t>Minimal Resource Requirements Test Plan</t>
+          <t>OTA Software Update Test Plan</t>
         </is>
       </c>
       <c r="C594" s="3" t="inlineStr">
         <is>
-          <t>[TC-RR-1.1] Minimal Resource Requirements for Matter Node</t>
+          <t>[TC-SU-4.2] Verifying Cluster Attributes from Admin(DUT)</t>
         </is>
       </c>
       <c r="D594" s="3" t="inlineStr">
         <is>
-          <t>TC-RR-1.1</t>
+          <t>TC-SU-4.2</t>
         </is>
       </c>
       <c r="E594" s="2" t="inlineStr">
@@ -15302,17 +15302,17 @@
       </c>
       <c r="B595" s="3" t="inlineStr">
         <is>
-          <t>System Model Test Plan</t>
+          <t>Access Control Enforcement Test Plan</t>
         </is>
       </c>
       <c r="C595" s="3" t="inlineStr">
         <is>
-          <t>[TC-SM-1.1] Device composition - Root Node [DUT as Server]</t>
+          <t>[TC-ACE-1.1] Privileges</t>
         </is>
       </c>
       <c r="D595" s="3" t="inlineStr">
         <is>
-          <t>TC-SM-1.1</t>
+          <t>TC-ACE-1.1</t>
         </is>
       </c>
       <c r="E595" s="2" t="inlineStr">
@@ -15327,20 +15327,220 @@
       </c>
       <c r="B596" s="3" t="inlineStr">
         <is>
+          <t>Access Control Enforcement Test Plan</t>
+        </is>
+      </c>
+      <c r="C596" s="3" t="inlineStr">
+        <is>
+          <t>[TC-ACE-1.2] Subscriptions</t>
+        </is>
+      </c>
+      <c r="D596" s="3" t="inlineStr">
+        <is>
+          <t>TC-ACE-1.2</t>
+        </is>
+      </c>
+      <c r="E596" s="2" t="inlineStr">
+        <is>
+          <t>Core Test Case</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" s="2" t="n">
+        <v>597</v>
+      </c>
+      <c r="B597" s="3" t="inlineStr">
+        <is>
+          <t>Access Control Enforcement Test Plan</t>
+        </is>
+      </c>
+      <c r="C597" s="3" t="inlineStr">
+        <is>
+          <t>[TC-ACE-1.3] Subjects</t>
+        </is>
+      </c>
+      <c r="D597" s="3" t="inlineStr">
+        <is>
+          <t>TC-ACE-1.3</t>
+        </is>
+      </c>
+      <c r="E597" s="2" t="inlineStr">
+        <is>
+          <t>Core Test Case</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" s="2" t="n">
+        <v>598</v>
+      </c>
+      <c r="B598" s="3" t="inlineStr">
+        <is>
+          <t>Access Control Enforcement Test Plan</t>
+        </is>
+      </c>
+      <c r="C598" s="3" t="inlineStr">
+        <is>
+          <t>[TC-ACE-1.4] Targets</t>
+        </is>
+      </c>
+      <c r="D598" s="3" t="inlineStr">
+        <is>
+          <t>TC-ACE-1.4</t>
+        </is>
+      </c>
+      <c r="E598" s="2" t="inlineStr">
+        <is>
+          <t>Core Test Case</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" s="2" t="n">
+        <v>599</v>
+      </c>
+      <c r="B599" s="3" t="inlineStr">
+        <is>
+          <t>Access Control Enforcement Test Plan</t>
+        </is>
+      </c>
+      <c r="C599" s="3" t="inlineStr">
+        <is>
+          <t>[TC-ACE-1.5] Multi-fabric</t>
+        </is>
+      </c>
+      <c r="D599" s="3" t="inlineStr">
+        <is>
+          <t>TC-ACE-1.5</t>
+        </is>
+      </c>
+      <c r="E599" s="2" t="inlineStr">
+        <is>
+          <t>Core Test Case</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" s="2" t="n">
+        <v>600</v>
+      </c>
+      <c r="B600" s="3" t="inlineStr">
+        <is>
+          <t>Access Control Enforcement Test Plan</t>
+        </is>
+      </c>
+      <c r="C600" s="3" t="inlineStr">
+        <is>
+          <t>[TC-ACE-1.6] Group auth mode</t>
+        </is>
+      </c>
+      <c r="D600" s="3" t="inlineStr">
+        <is>
+          <t>TC-ACE-1.6</t>
+        </is>
+      </c>
+      <c r="E600" s="2" t="inlineStr">
+        <is>
+          <t>Core Test Case</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" s="2" t="n">
+        <v>601</v>
+      </c>
+      <c r="B601" s="3" t="inlineStr">
+        <is>
+          <t>Minimal Resource Requirements Test Plan</t>
+        </is>
+      </c>
+      <c r="C601" s="3" t="inlineStr">
+        <is>
+          <t>[TC-RR-1.1] Minimal Resource Requirements for Matter Node</t>
+        </is>
+      </c>
+      <c r="D601" s="3" t="inlineStr">
+        <is>
+          <t>TC-RR-1.1</t>
+        </is>
+      </c>
+      <c r="E601" s="2" t="inlineStr">
+        <is>
+          <t>Core Test Case</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" s="2" t="n">
+        <v>602</v>
+      </c>
+      <c r="B602" s="3" t="inlineStr">
+        <is>
           <t>System Model Test Plan</t>
         </is>
       </c>
-      <c r="C596" s="3" t="inlineStr">
+      <c r="C602" s="3" t="inlineStr">
+        <is>
+          <t>[TC-SM-1.1] Device composition - Root Node [DUT as Server]</t>
+        </is>
+      </c>
+      <c r="D602" s="3" t="inlineStr">
+        <is>
+          <t>TC-SM-1.1</t>
+        </is>
+      </c>
+      <c r="E602" s="2" t="inlineStr">
+        <is>
+          <t>Core Test Case</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" s="2" t="n">
+        <v>603</v>
+      </c>
+      <c r="B603" s="3" t="inlineStr">
+        <is>
+          <t>System Model Test Plan</t>
+        </is>
+      </c>
+      <c r="C603" s="3" t="inlineStr">
         <is>
           <t>[TC-SM-1.2] Device composition - Topology [DUT as Server]</t>
         </is>
       </c>
-      <c r="D596" s="3" t="inlineStr">
+      <c r="D603" s="3" t="inlineStr">
         <is>
           <t>TC-SM-1.2</t>
         </is>
       </c>
-      <c r="E596" s="2" t="inlineStr">
+      <c r="E603" s="2" t="inlineStr">
+        <is>
+          <t>Core Test Case</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" s="2" t="n">
+        <v>604</v>
+      </c>
+      <c r="B604" s="3" t="inlineStr">
+        <is>
+          <t>Device Types Test Plan</t>
+        </is>
+      </c>
+      <c r="C604" s="3" t="inlineStr">
+        <is>
+          <t>[TC-DT-1.1] Base Device Type [DUT as Server]</t>
+        </is>
+      </c>
+      <c r="D604" s="3" t="inlineStr">
+        <is>
+          <t>TC-DT-1.1</t>
+        </is>
+      </c>
+      <c r="E604" s="2" t="inlineStr">
         <is>
           <t>Core Test Case</t>
         </is>

</xml_diff>